<commit_message>
Herramienta de Gestion de la calidad 1.0
</commit_message>
<xml_diff>
--- a/PPQA/Resolucion/HGQA_V1.0_2017.xlsx
+++ b/PPQA/Resolucion/HGQA_V1.0_2017.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" tabRatio="642"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="642" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Historial de Revisiones" sheetId="14" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <externalReference r:id="rId7"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Planificación!$A$12:$Y$45</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Planificación!$A$12:$Y$47</definedName>
     <definedName name="Analista" localSheetId="0">#REF!</definedName>
     <definedName name="AreaProceso" localSheetId="0">#REF!</definedName>
     <definedName name="Artefacto" localSheetId="0">#REF!</definedName>
@@ -168,7 +168,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="249">
   <si>
     <t>Analista Responsable</t>
   </si>
@@ -688,9 +688,6 @@
     <t>Miguel Cotrina - Luis Torres</t>
   </si>
   <si>
-    <t>Plan de proyecto</t>
-  </si>
-  <si>
     <t>Diego Sebastian</t>
   </si>
   <si>
@@ -718,75 +715,12 @@
     <t>CM</t>
   </si>
   <si>
-    <t>Cronograma de proyecto</t>
-  </si>
-  <si>
-    <t>Proceso de gestion de proyecto</t>
-  </si>
-  <si>
     <t>Sebastian Diego</t>
   </si>
   <si>
-    <t>Aceptacion de entregables</t>
-  </si>
-  <si>
     <t>Junio Trillo</t>
   </si>
   <si>
-    <t>Registro de riesgos</t>
-  </si>
-  <si>
-    <t>Registro de Items de configuracion</t>
-  </si>
-  <si>
-    <t>Formato de solicitud de accesos</t>
-  </si>
-  <si>
-    <t>Proceso de gestion de configuracion</t>
-  </si>
-  <si>
-    <t>Ficha de métricas de índice de cambios en ítems de configuración</t>
-  </si>
-  <si>
-    <t>Ficha de métricas de volatilidad de requerimientos</t>
-  </si>
-  <si>
-    <t>CheckList de aseguramiento de la calidad</t>
-  </si>
-  <si>
-    <t>Herramienta de gestión de aseguramiento de calidad</t>
-  </si>
-  <si>
-    <t>Matriz de seguimiento de proyecto interno</t>
-  </si>
-  <si>
-    <t>Proceso de aseguramiento de calidad</t>
-  </si>
-  <si>
-    <t>Fichas de métricas de numero de N conformidades QA del producto</t>
-  </si>
-  <si>
-    <t>Solicitud de cambios a requerimientos</t>
-  </si>
-  <si>
-    <t>Matriz de trazabilidad de requerimientos</t>
-  </si>
-  <si>
-    <t>Proceso de gestión de requerimientos</t>
-  </si>
-  <si>
-    <t>Registro de cambios a requerimientos</t>
-  </si>
-  <si>
-    <t>Lista maestra de requerimientos</t>
-  </si>
-  <si>
-    <t>Acta de reuniones</t>
-  </si>
-  <si>
-    <t>Avance Quincenales</t>
-  </si>
-  <si>
     <t>Fecha Efectiva: 15/06/2017</t>
   </si>
   <si>
@@ -808,9 +742,6 @@
     <t>No se encontro disconformidad</t>
   </si>
   <si>
-    <t>No disconformidad</t>
-  </si>
-  <si>
     <t xml:space="preserve">Entregable </t>
   </si>
   <si>
@@ -820,9 +751,6 @@
     <t>Manuel Tarazona</t>
   </si>
   <si>
-    <t>Posee defectos en las subcarpetas</t>
-  </si>
-  <si>
     <t>Los subprocesos no tienen los roles correctamente definidos, las funciones de cada rol no son las correctas</t>
   </si>
   <si>
@@ -889,12 +817,6 @@
     <t>La seccion instructivo tiene un pequeño defecto de formato</t>
   </si>
   <si>
-    <t>Se encontro preguntas redundantes en la seccion de CM y PP-PMC</t>
-  </si>
-  <si>
-    <t>Se encontro un par de errores en la seccion planificacion / Fecha fin real</t>
-  </si>
-  <si>
     <t>La seccion REQ a DOC esta incompleta</t>
   </si>
   <si>
@@ -911,6 +833,96 @@
   </si>
   <si>
     <t>Solo se encontro un pequeño error en el formato de las tablas</t>
+  </si>
+  <si>
+    <t>Plan de proyecto (PPROY)</t>
+  </si>
+  <si>
+    <t>Acta de reuniones (ARINT- AREXT)</t>
+  </si>
+  <si>
+    <t>Cronograma de proyecto (CPROY)</t>
+  </si>
+  <si>
+    <t>Proceso de gestion de proyecto (PGPROY)</t>
+  </si>
+  <si>
+    <t>Aceptacion de entregables (ACENTRE)</t>
+  </si>
+  <si>
+    <t>Avance Quincenales (IAVQUI)</t>
+  </si>
+  <si>
+    <t>Registro de riesgos (REGRI)</t>
+  </si>
+  <si>
+    <t>Registro de Items de configuracion (REGITCON)</t>
+  </si>
+  <si>
+    <t>Formato de solicitud de accesos (SOLACC)</t>
+  </si>
+  <si>
+    <t>Proceso de gestion de configuracion (PGC)</t>
+  </si>
+  <si>
+    <t>Ficha de métricas de índice de cambios en ítems de configuración (FMICIC)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ficha de métricas de volatilidad de requerimientos (FMVREQM)</t>
+  </si>
+  <si>
+    <t>CheckList de aseguramiento de la calidad (CHKQA)</t>
+  </si>
+  <si>
+    <t>Herramienta de gestión de aseguramiento de calidad (HGQA)</t>
+  </si>
+  <si>
+    <t>Matriz de seguimiento de proyecto interno (MSPQA)</t>
+  </si>
+  <si>
+    <t>Proceso de aseguramiento de calidad (PQA)</t>
+  </si>
+  <si>
+    <t>Fichas de métricas de numero de N conformidades QA del producto (FMNCONPRO)</t>
+  </si>
+  <si>
+    <t>Solicitud de cambios a requerimientos (SOLCREQ)</t>
+  </si>
+  <si>
+    <t>Matriz de trazabilidad de requerimientos (MTREQM)</t>
+  </si>
+  <si>
+    <t>Proceso de gestión de requerimientos (PGREQM)</t>
+  </si>
+  <si>
+    <t>Registro de cambios a requerimientos (RCREQM)</t>
+  </si>
+  <si>
+    <t>Lista maestra de requerimientos (LMR)</t>
+  </si>
+  <si>
+    <t>Fichas de métricas de exposicion al riesgo (FMEXRI)</t>
+  </si>
+  <si>
+    <t>Tablero de metricas (TMETR)</t>
+  </si>
+  <si>
+    <t>Se encontro fechas que no coinciden. Errrores en el seguimiento de nc. Los entregables no tienen su nomenclatura</t>
+  </si>
+  <si>
+    <t>Se encontro preguntas redundantes y poco explicitas en todas las secciones</t>
+  </si>
+  <si>
+    <t>El historial de revisiones esta incorrecto</t>
+  </si>
+  <si>
+    <t>Existe errores en los roles de trabajo. Los procesos tienen informacion que no corresponde al plan de proyecto</t>
+  </si>
+  <si>
+    <t>Se encontro un par de errores en la seccion planificacion / Fecha fin real. Los procesos no estan definidos correctamente</t>
+  </si>
+  <si>
+    <t>Posee defectos en las rutas de subcarpetas</t>
   </si>
 </sst>
 </file>
@@ -2453,6 +2465,17 @@
     <xf numFmtId="0" fontId="13" fillId="28" borderId="10" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="24" borderId="29" xfId="39" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="11" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="44" fillId="24" borderId="0" xfId="43" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2465,15 +2488,51 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="29" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="11" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="33" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="29" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="11" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="33" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="29" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="33" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="29" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="33" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="29" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2483,6 +2542,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2504,41 +2566,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="32" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="11" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="33" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="29" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="11" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="33" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="29" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="11" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="33" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="29" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="24" borderId="0" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="25" borderId="11" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -2548,26 +2594,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="11" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="33" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="29" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="24" borderId="0" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="44" fillId="24" borderId="34" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -2580,6 +2606,34 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="44" fillId="24" borderId="0" xfId="32" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="25" borderId="10" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="24" borderId="11" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="24" borderId="33" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="24" borderId="29" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="25" borderId="11" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="25" borderId="29" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="49" fontId="56" fillId="25" borderId="10" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2591,18 +2645,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="24" borderId="11" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="24" borderId="33" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="24" borderId="29" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="52" fillId="25" borderId="10" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -2631,22 +2673,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="24" borderId="0" xfId="32" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="25" borderId="10" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="25" borderId="11" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="25" borderId="29" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="10" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2658,20 +2684,6 @@
     </xf>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="40" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="24" borderId="29" xfId="39" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="11" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="53">
@@ -2919,7 +2931,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3321,9 +3333,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Informe de Revisión'!$C$28:$C$32</c:f>
+              <c:f>'Informe de Revisión'!$C$28:$C$31</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>Documento</c:v>
                 </c:pt>
@@ -3336,32 +3348,26 @@
                 <c:pt idx="3">
                   <c:v>Control de Configuración</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>No disconformidad</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Informe de Revisión'!$D$28:$D$32</c:f>
+              <c:f>'Informe de Revisión'!$D$28:$D$31</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>9</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3546,7 +3552,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Informe de Revisión'!$C$42</c:f>
+              <c:f>'Informe de Revisión'!$C$41</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3666,7 +3672,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Informe de Revisión'!$C$40:$C$41</c:f>
+              <c:f>'Informe de Revisión'!$C$39:$C$40</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -3680,15 +3686,15 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Informe de Revisión'!$D$40:$D$41</c:f>
+              <c:f>'Informe de Revisión'!$D$39:$D$40</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>30.2</c:v>
+                  <c:v>32.800000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29.400000000000002</c:v>
+                  <c:v>31.400000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4024,7 +4030,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Informe de Revisión'!$C$58</c:f>
+              <c:f>'Informe de Revisión'!$C$57</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4084,12 +4090,12 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>'Informe de Revisión'!$D$58</c:f>
+              <c:f>'Informe de Revisión'!$D$57</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>21</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4105,7 +4111,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Informe de Revisión'!$C$59</c:f>
+              <c:f>'Informe de Revisión'!$C$58</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4165,7 +4171,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>'Informe de Revisión'!$D$59</c:f>
+              <c:f>'Informe de Revisión'!$D$58</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
@@ -4186,7 +4192,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Informe de Revisión'!$C$60</c:f>
+              <c:f>'Informe de Revisión'!$C$59</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4246,7 +4252,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>'Informe de Revisión'!$D$60</c:f>
+              <c:f>'Informe de Revisión'!$D$59</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
@@ -4777,7 +4783,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4809,13 +4815,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4847,13 +4853,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>65</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5277,7 +5283,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -5307,15 +5313,15 @@
     </row>
     <row r="2" spans="1:9" ht="15.75">
       <c r="A2" s="66"/>
-      <c r="B2" s="142" t="s">
+      <c r="B2" s="146" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="142"/>
-      <c r="D2" s="142"/>
-      <c r="E2" s="142"/>
-      <c r="F2" s="142"/>
-      <c r="G2" s="142"/>
-      <c r="H2" s="142"/>
+      <c r="C2" s="146"/>
+      <c r="D2" s="146"/>
+      <c r="E2" s="146"/>
+      <c r="F2" s="146"/>
+      <c r="G2" s="146"/>
+      <c r="H2" s="146"/>
       <c r="I2" s="66"/>
     </row>
     <row r="3" spans="1:9" ht="13.5" thickBot="1">
@@ -5375,7 +5381,7 @@
         <v>69</v>
       </c>
       <c r="H5" s="76" t="s">
-        <v>213</v>
+        <v>190</v>
       </c>
       <c r="I5" s="66"/>
     </row>
@@ -5466,22 +5472,22 @@
     <row r="2" spans="1:8" s="62" customFormat="1" ht="48.75" customHeight="1">
       <c r="A2" s="40"/>
       <c r="B2"/>
-      <c r="C2" s="149" t="s">
+      <c r="C2" s="165" t="s">
         <v>162</v>
       </c>
-      <c r="D2" s="150"/>
-      <c r="E2" s="151"/>
+      <c r="D2" s="166"/>
+      <c r="E2" s="167"/>
     </row>
     <row r="3" spans="1:8" s="62" customFormat="1">
       <c r="A3" s="40"/>
       <c r="B3" s="63" t="s">
         <v>93</v>
       </c>
-      <c r="C3" s="156" t="s">
-        <v>203</v>
-      </c>
-      <c r="D3" s="157"/>
-      <c r="E3" s="158"/>
+      <c r="C3" s="173" t="s">
+        <v>181</v>
+      </c>
+      <c r="D3" s="174"/>
+      <c r="E3" s="175"/>
     </row>
     <row r="4" spans="1:8" s="62" customFormat="1" ht="21.75" customHeight="1">
       <c r="A4" s="40"/>
@@ -5493,12 +5499,12 @@
     </row>
     <row r="5" spans="1:8" ht="24.75" customHeight="1">
       <c r="A5" s="40"/>
-      <c r="B5" s="205" t="s">
-        <v>218</v>
-      </c>
-      <c r="C5" s="152"/>
-      <c r="D5" s="152"/>
-      <c r="E5" s="153"/>
+      <c r="B5" s="168" t="s">
+        <v>194</v>
+      </c>
+      <c r="C5" s="169"/>
+      <c r="D5" s="169"/>
+      <c r="E5" s="170"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="40"/>
@@ -5521,10 +5527,10 @@
         <v>5</v>
       </c>
       <c r="C8" s="91"/>
-      <c r="D8" s="154" t="s">
+      <c r="D8" s="171" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="155"/>
+      <c r="E8" s="172"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="40"/>
@@ -5610,22 +5616,22 @@
       <c r="A18" s="38"/>
     </row>
     <row r="19" spans="1:8" s="58" customFormat="1" ht="16.5" customHeight="1">
-      <c r="B19" s="162" t="s">
+      <c r="B19" s="153" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="163"/>
-      <c r="D19" s="163"/>
-      <c r="E19" s="164"/>
+      <c r="C19" s="154"/>
+      <c r="D19" s="154"/>
+      <c r="E19" s="155"/>
     </row>
     <row r="20" spans="1:8" s="58" customFormat="1" ht="13.5" customHeight="1">
       <c r="B20" s="141" t="s">
         <v>70</v>
       </c>
-      <c r="C20" s="165" t="s">
+      <c r="C20" s="156" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="166"/>
-      <c r="E20" s="167"/>
+      <c r="D20" s="157"/>
+      <c r="E20" s="158"/>
     </row>
     <row r="21" spans="1:8" s="58" customFormat="1" ht="12.75" customHeight="1">
       <c r="B21" s="59" t="s">
@@ -5678,31 +5684,31 @@
       <c r="B26" s="51"/>
     </row>
     <row r="27" spans="1:8" s="58" customFormat="1" ht="16.5" customHeight="1">
-      <c r="B27" s="162" t="s">
+      <c r="B27" s="153" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="163"/>
-      <c r="D27" s="163"/>
-      <c r="E27" s="164"/>
+      <c r="C27" s="154"/>
+      <c r="D27" s="154"/>
+      <c r="E27" s="155"/>
     </row>
     <row r="28" spans="1:8" s="58" customFormat="1" ht="13.5" customHeight="1">
       <c r="B28" s="141" t="s">
         <v>70</v>
       </c>
-      <c r="C28" s="165" t="s">
+      <c r="C28" s="156" t="s">
         <v>6</v>
       </c>
-      <c r="D28" s="166"/>
-      <c r="E28" s="167"/>
+      <c r="D28" s="157"/>
+      <c r="E28" s="158"/>
     </row>
     <row r="29" spans="1:8" ht="12.75" customHeight="1">
       <c r="A29" s="38"/>
-      <c r="B29" s="168" t="s">
+      <c r="B29" s="150" t="s">
         <v>50</v>
       </c>
-      <c r="C29" s="169"/>
-      <c r="D29" s="169"/>
-      <c r="E29" s="170"/>
+      <c r="C29" s="151"/>
+      <c r="D29" s="151"/>
+      <c r="E29" s="152"/>
       <c r="F29" s="58"/>
       <c r="G29" s="58"/>
     </row>
@@ -5711,11 +5717,11 @@
       <c r="B30" s="48" t="s">
         <v>163</v>
       </c>
-      <c r="C30" s="143" t="s">
+      <c r="C30" s="147" t="s">
         <v>165</v>
       </c>
-      <c r="D30" s="144"/>
-      <c r="E30" s="145"/>
+      <c r="D30" s="148"/>
+      <c r="E30" s="149"/>
       <c r="F30" s="58"/>
       <c r="G30" s="58"/>
     </row>
@@ -5724,11 +5730,11 @@
       <c r="B31" s="46" t="s">
         <v>164</v>
       </c>
-      <c r="C31" s="143" t="s">
+      <c r="C31" s="147" t="s">
         <v>166</v>
       </c>
-      <c r="D31" s="144"/>
-      <c r="E31" s="145"/>
+      <c r="D31" s="148"/>
+      <c r="E31" s="149"/>
       <c r="F31" s="58"/>
       <c r="G31" s="58"/>
     </row>
@@ -5737,11 +5743,11 @@
       <c r="B32" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="143" t="s">
+      <c r="C32" s="147" t="s">
         <v>53</v>
       </c>
-      <c r="D32" s="144"/>
-      <c r="E32" s="145"/>
+      <c r="D32" s="148"/>
+      <c r="E32" s="149"/>
       <c r="F32" s="58"/>
       <c r="G32" s="58"/>
     </row>
@@ -5750,11 +5756,11 @@
       <c r="B33" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="C33" s="143" t="s">
+      <c r="C33" s="147" t="s">
         <v>71</v>
       </c>
-      <c r="D33" s="144"/>
-      <c r="E33" s="145"/>
+      <c r="D33" s="148"/>
+      <c r="E33" s="149"/>
       <c r="F33" s="58"/>
       <c r="G33" s="58"/>
     </row>
@@ -5763,174 +5769,174 @@
       <c r="B34" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C34" s="143" t="s">
+      <c r="C34" s="147" t="s">
         <v>72</v>
       </c>
-      <c r="D34" s="144"/>
-      <c r="E34" s="145"/>
+      <c r="D34" s="148"/>
+      <c r="E34" s="149"/>
     </row>
     <row r="35" spans="1:7" ht="16.5" customHeight="1">
       <c r="A35" s="38"/>
       <c r="B35" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="C35" s="143" t="s">
+      <c r="C35" s="147" t="s">
         <v>73</v>
       </c>
-      <c r="D35" s="144"/>
-      <c r="E35" s="145"/>
+      <c r="D35" s="148"/>
+      <c r="E35" s="149"/>
     </row>
     <row r="36" spans="1:7" ht="16.5" customHeight="1">
       <c r="A36" s="38"/>
-      <c r="B36" s="168" t="s">
+      <c r="B36" s="150" t="s">
         <v>51</v>
       </c>
-      <c r="C36" s="169"/>
-      <c r="D36" s="169"/>
-      <c r="E36" s="170"/>
+      <c r="C36" s="151"/>
+      <c r="D36" s="151"/>
+      <c r="E36" s="152"/>
     </row>
     <row r="37" spans="1:7" ht="16.5" customHeight="1">
       <c r="A37" s="38"/>
       <c r="B37" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="143" t="s">
+      <c r="C37" s="147" t="s">
         <v>74</v>
       </c>
-      <c r="D37" s="144"/>
-      <c r="E37" s="145"/>
+      <c r="D37" s="148"/>
+      <c r="E37" s="149"/>
     </row>
     <row r="38" spans="1:7" ht="16.5" customHeight="1">
       <c r="A38" s="38"/>
       <c r="B38" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="C38" s="143" t="s">
+      <c r="C38" s="147" t="s">
         <v>85</v>
       </c>
-      <c r="D38" s="144"/>
-      <c r="E38" s="145"/>
+      <c r="D38" s="148"/>
+      <c r="E38" s="149"/>
     </row>
     <row r="39" spans="1:7" ht="17.25" customHeight="1">
       <c r="A39" s="38"/>
       <c r="B39" s="46" t="s">
         <v>101</v>
       </c>
-      <c r="C39" s="143" t="s">
+      <c r="C39" s="147" t="s">
         <v>102</v>
       </c>
-      <c r="D39" s="144"/>
-      <c r="E39" s="145"/>
+      <c r="D39" s="148"/>
+      <c r="E39" s="149"/>
     </row>
     <row r="40" spans="1:7" ht="16.5" customHeight="1">
       <c r="A40" s="38"/>
       <c r="B40" s="46" t="s">
         <v>143</v>
       </c>
-      <c r="C40" s="143" t="s">
+      <c r="C40" s="147" t="s">
         <v>144</v>
       </c>
-      <c r="D40" s="144"/>
-      <c r="E40" s="145"/>
+      <c r="D40" s="148"/>
+      <c r="E40" s="149"/>
     </row>
     <row r="41" spans="1:7" ht="16.5" customHeight="1">
       <c r="A41" s="38"/>
       <c r="B41" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C41" s="143" t="s">
+      <c r="C41" s="147" t="s">
         <v>104</v>
       </c>
-      <c r="D41" s="144"/>
-      <c r="E41" s="145"/>
+      <c r="D41" s="148"/>
+      <c r="E41" s="149"/>
     </row>
     <row r="42" spans="1:7" ht="16.5" customHeight="1">
       <c r="A42" s="38"/>
       <c r="B42" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="C42" s="143" t="s">
+      <c r="C42" s="147" t="s">
         <v>103</v>
       </c>
-      <c r="D42" s="144"/>
-      <c r="E42" s="145"/>
+      <c r="D42" s="148"/>
+      <c r="E42" s="149"/>
     </row>
     <row r="43" spans="1:7" ht="16.5" customHeight="1">
       <c r="A43" s="38"/>
       <c r="B43" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="C43" s="143" t="s">
+      <c r="C43" s="147" t="s">
         <v>77</v>
       </c>
-      <c r="D43" s="144"/>
-      <c r="E43" s="145"/>
+      <c r="D43" s="148"/>
+      <c r="E43" s="149"/>
     </row>
     <row r="44" spans="1:7" ht="16.5" customHeight="1">
       <c r="A44" s="38"/>
       <c r="B44" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="C44" s="143" t="s">
+      <c r="C44" s="147" t="s">
         <v>78</v>
       </c>
-      <c r="D44" s="144"/>
-      <c r="E44" s="145"/>
+      <c r="D44" s="148"/>
+      <c r="E44" s="149"/>
     </row>
     <row r="45" spans="1:7" ht="16.5" customHeight="1">
       <c r="A45" s="38"/>
       <c r="B45" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="C45" s="143" t="s">
+      <c r="C45" s="147" t="s">
         <v>75</v>
       </c>
-      <c r="D45" s="144"/>
-      <c r="E45" s="145"/>
+      <c r="D45" s="148"/>
+      <c r="E45" s="149"/>
     </row>
     <row r="46" spans="1:7" ht="16.5" customHeight="1">
       <c r="A46" s="38"/>
       <c r="B46" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="C46" s="143" t="s">
+      <c r="C46" s="147" t="s">
         <v>80</v>
       </c>
-      <c r="D46" s="144"/>
-      <c r="E46" s="145"/>
+      <c r="D46" s="148"/>
+      <c r="E46" s="149"/>
     </row>
     <row r="47" spans="1:7" ht="16.5" customHeight="1">
       <c r="A47" s="38"/>
       <c r="B47" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="C47" s="143" t="s">
+      <c r="C47" s="147" t="s">
         <v>81</v>
       </c>
-      <c r="D47" s="144"/>
-      <c r="E47" s="145"/>
+      <c r="D47" s="148"/>
+      <c r="E47" s="149"/>
     </row>
     <row r="48" spans="1:7" ht="16.5" customHeight="1">
       <c r="A48" s="38"/>
       <c r="B48" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="C48" s="143" t="s">
+      <c r="C48" s="147" t="s">
         <v>79</v>
       </c>
-      <c r="D48" s="144"/>
-      <c r="E48" s="145"/>
+      <c r="D48" s="148"/>
+      <c r="E48" s="149"/>
     </row>
     <row r="49" spans="1:13" ht="16.5" customHeight="1">
       <c r="A49" s="38"/>
       <c r="B49" s="46" t="s">
         <v>145</v>
       </c>
-      <c r="C49" s="143" t="s">
+      <c r="C49" s="147" t="s">
         <v>76</v>
       </c>
-      <c r="D49" s="144"/>
-      <c r="E49" s="145"/>
+      <c r="D49" s="148"/>
+      <c r="E49" s="149"/>
     </row>
     <row r="50" spans="1:13" ht="16.5" customHeight="1">
       <c r="A50" s="58"/>
@@ -5963,23 +5969,23 @@
       <c r="M51" s="39"/>
     </row>
     <row r="52" spans="1:13" s="58" customFormat="1" ht="16.5" customHeight="1">
-      <c r="B52" s="162" t="s">
+      <c r="B52" s="153" t="s">
         <v>54</v>
       </c>
-      <c r="C52" s="163"/>
-      <c r="D52" s="163"/>
-      <c r="E52" s="164"/>
+      <c r="C52" s="154"/>
+      <c r="D52" s="154"/>
+      <c r="E52" s="155"/>
     </row>
     <row r="53" spans="1:13" ht="16.5" customHeight="1">
       <c r="A53" s="58"/>
       <c r="B53" s="141" t="s">
         <v>47</v>
       </c>
-      <c r="C53" s="165" t="s">
+      <c r="C53" s="156" t="s">
         <v>6</v>
       </c>
-      <c r="D53" s="166"/>
-      <c r="E53" s="167"/>
+      <c r="D53" s="157"/>
+      <c r="E53" s="158"/>
       <c r="F53" s="58"/>
       <c r="G53" s="58"/>
       <c r="H53" s="58"/>
@@ -5994,132 +6000,132 @@
       <c r="B54" s="46" t="s">
         <v>146</v>
       </c>
-      <c r="C54" s="143" t="s">
+      <c r="C54" s="147" t="s">
         <v>74</v>
       </c>
-      <c r="D54" s="144"/>
-      <c r="E54" s="145"/>
+      <c r="D54" s="148"/>
+      <c r="E54" s="149"/>
     </row>
     <row r="55" spans="1:13" ht="16.5" customHeight="1">
       <c r="A55" s="38"/>
       <c r="B55" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="C55" s="143" t="s">
+      <c r="C55" s="147" t="s">
         <v>86</v>
       </c>
-      <c r="D55" s="144"/>
-      <c r="E55" s="145"/>
+      <c r="D55" s="148"/>
+      <c r="E55" s="149"/>
     </row>
     <row r="56" spans="1:13" ht="16.5" customHeight="1">
       <c r="A56" s="38"/>
       <c r="B56" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="C56" s="143" t="s">
+      <c r="C56" s="147" t="s">
         <v>87</v>
       </c>
-      <c r="D56" s="144"/>
-      <c r="E56" s="145"/>
+      <c r="D56" s="148"/>
+      <c r="E56" s="149"/>
     </row>
     <row r="57" spans="1:13" ht="16.5" customHeight="1">
       <c r="A57" s="38"/>
       <c r="B57" s="46" t="s">
         <v>111</v>
       </c>
-      <c r="C57" s="143" t="s">
+      <c r="C57" s="147" t="s">
         <v>105</v>
       </c>
-      <c r="D57" s="147"/>
-      <c r="E57" s="148"/>
+      <c r="D57" s="162"/>
+      <c r="E57" s="163"/>
     </row>
     <row r="58" spans="1:13" ht="16.5" customHeight="1">
       <c r="A58" s="38"/>
       <c r="B58" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="C58" s="143" t="s">
+      <c r="C58" s="147" t="s">
         <v>91</v>
       </c>
-      <c r="D58" s="147"/>
-      <c r="E58" s="148"/>
+      <c r="D58" s="162"/>
+      <c r="E58" s="163"/>
     </row>
     <row r="59" spans="1:13" ht="16.5" customHeight="1">
       <c r="A59" s="38"/>
       <c r="B59" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="C59" s="143" t="s">
+      <c r="C59" s="147" t="s">
         <v>82</v>
       </c>
-      <c r="D59" s="147"/>
-      <c r="E59" s="148"/>
+      <c r="D59" s="162"/>
+      <c r="E59" s="163"/>
     </row>
     <row r="60" spans="1:13" ht="54" customHeight="1">
       <c r="A60" s="38"/>
       <c r="B60" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="C60" s="143" t="s">
+      <c r="C60" s="147" t="s">
         <v>106</v>
       </c>
-      <c r="D60" s="147"/>
-      <c r="E60" s="148"/>
+      <c r="D60" s="162"/>
+      <c r="E60" s="163"/>
     </row>
     <row r="61" spans="1:13" ht="16.5" customHeight="1">
       <c r="A61" s="38"/>
       <c r="B61" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="C61" s="146" t="s">
+      <c r="C61" s="164" t="s">
         <v>90</v>
       </c>
-      <c r="D61" s="147"/>
-      <c r="E61" s="148"/>
+      <c r="D61" s="162"/>
+      <c r="E61" s="163"/>
     </row>
     <row r="62" spans="1:13" ht="30" customHeight="1">
       <c r="A62" s="38"/>
       <c r="B62" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="C62" s="143" t="s">
+      <c r="C62" s="147" t="s">
         <v>56</v>
       </c>
-      <c r="D62" s="147"/>
-      <c r="E62" s="148"/>
+      <c r="D62" s="162"/>
+      <c r="E62" s="163"/>
     </row>
     <row r="63" spans="1:13" ht="16.5" customHeight="1">
       <c r="A63" s="38"/>
       <c r="B63" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="C63" s="146" t="s">
+      <c r="C63" s="164" t="s">
         <v>61</v>
       </c>
-      <c r="D63" s="147"/>
-      <c r="E63" s="148"/>
+      <c r="D63" s="162"/>
+      <c r="E63" s="163"/>
     </row>
     <row r="64" spans="1:13" ht="16.5" customHeight="1">
       <c r="A64" s="38"/>
       <c r="B64" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="C64" s="146" t="s">
+      <c r="C64" s="164" t="s">
         <v>83</v>
       </c>
-      <c r="D64" s="147"/>
-      <c r="E64" s="148"/>
+      <c r="D64" s="162"/>
+      <c r="E64" s="163"/>
     </row>
     <row r="65" spans="1:8" ht="16.5" customHeight="1">
       <c r="A65" s="38"/>
       <c r="B65" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="C65" s="143" t="s">
+      <c r="C65" s="147" t="s">
         <v>76</v>
       </c>
-      <c r="D65" s="144"/>
-      <c r="E65" s="145"/>
+      <c r="D65" s="148"/>
+      <c r="E65" s="149"/>
     </row>
     <row r="66" spans="1:8" ht="16.5" customHeight="1">
       <c r="A66" s="38"/>
@@ -6130,12 +6136,12 @@
     </row>
     <row r="67" spans="1:8" ht="16.5" customHeight="1">
       <c r="A67" s="38"/>
-      <c r="B67" s="162" t="s">
-        <v>219</v>
-      </c>
-      <c r="C67" s="163"/>
-      <c r="D67" s="163"/>
-      <c r="E67" s="164"/>
+      <c r="B67" s="153" t="s">
+        <v>195</v>
+      </c>
+      <c r="C67" s="154"/>
+      <c r="D67" s="154"/>
+      <c r="E67" s="155"/>
       <c r="F67" s="57"/>
       <c r="G67" s="57"/>
       <c r="H67" s="57"/>
@@ -6145,23 +6151,23 @@
       <c r="B68" s="141" t="s">
         <v>70</v>
       </c>
-      <c r="C68" s="165" t="s">
+      <c r="C68" s="156" t="s">
         <v>6</v>
       </c>
-      <c r="D68" s="166"/>
-      <c r="E68" s="167"/>
+      <c r="D68" s="157"/>
+      <c r="E68" s="158"/>
       <c r="F68" s="57"/>
       <c r="G68" s="57"/>
       <c r="H68" s="57"/>
     </row>
     <row r="69" spans="1:8" ht="16.5" customHeight="1">
       <c r="A69" s="38"/>
-      <c r="B69" s="168" t="s">
+      <c r="B69" s="150" t="s">
         <v>50</v>
       </c>
-      <c r="C69" s="169"/>
-      <c r="D69" s="169"/>
-      <c r="E69" s="170"/>
+      <c r="C69" s="151"/>
+      <c r="D69" s="151"/>
+      <c r="E69" s="152"/>
       <c r="F69" s="57"/>
       <c r="G69" s="57"/>
       <c r="H69" s="57"/>
@@ -6171,11 +6177,11 @@
       <c r="B70" s="48" t="s">
         <v>163</v>
       </c>
-      <c r="C70" s="143" t="s">
+      <c r="C70" s="147" t="s">
         <v>165</v>
       </c>
-      <c r="D70" s="144"/>
-      <c r="E70" s="145"/>
+      <c r="D70" s="148"/>
+      <c r="E70" s="149"/>
       <c r="F70" s="57"/>
       <c r="G70" s="57"/>
       <c r="H70" s="57"/>
@@ -6185,11 +6191,11 @@
       <c r="B71" s="46" t="s">
         <v>164</v>
       </c>
-      <c r="C71" s="143" t="s">
+      <c r="C71" s="147" t="s">
         <v>166</v>
       </c>
-      <c r="D71" s="144"/>
-      <c r="E71" s="145"/>
+      <c r="D71" s="148"/>
+      <c r="E71" s="149"/>
       <c r="F71" s="57"/>
       <c r="G71" s="57"/>
       <c r="H71" s="57"/>
@@ -6199,11 +6205,11 @@
       <c r="B72" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="C72" s="143" t="s">
+      <c r="C72" s="147" t="s">
         <v>53</v>
       </c>
-      <c r="D72" s="144"/>
-      <c r="E72" s="145"/>
+      <c r="D72" s="148"/>
+      <c r="E72" s="149"/>
       <c r="F72" s="57"/>
       <c r="G72" s="57"/>
       <c r="H72" s="57"/>
@@ -6213,11 +6219,11 @@
       <c r="B73" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="C73" s="143" t="s">
+      <c r="C73" s="147" t="s">
         <v>71</v>
       </c>
-      <c r="D73" s="144"/>
-      <c r="E73" s="145"/>
+      <c r="D73" s="148"/>
+      <c r="E73" s="149"/>
       <c r="F73" s="57"/>
       <c r="G73" s="57"/>
       <c r="H73" s="57"/>
@@ -6227,11 +6233,11 @@
       <c r="B74" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C74" s="143" t="s">
+      <c r="C74" s="147" t="s">
         <v>72</v>
       </c>
-      <c r="D74" s="144"/>
-      <c r="E74" s="145"/>
+      <c r="D74" s="148"/>
+      <c r="E74" s="149"/>
       <c r="F74" s="57"/>
       <c r="G74" s="57"/>
       <c r="H74" s="57"/>
@@ -6241,93 +6247,93 @@
       <c r="B75" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="C75" s="143" t="s">
+      <c r="C75" s="147" t="s">
         <v>73</v>
       </c>
-      <c r="D75" s="144"/>
-      <c r="E75" s="145"/>
+      <c r="D75" s="148"/>
+      <c r="E75" s="149"/>
       <c r="F75" s="57"/>
       <c r="G75" s="57"/>
       <c r="H75" s="57"/>
     </row>
     <row r="76" spans="1:8" ht="16.5" customHeight="1">
       <c r="A76" s="38"/>
-      <c r="B76" s="168" t="s">
+      <c r="B76" s="150" t="s">
         <v>51</v>
       </c>
-      <c r="C76" s="169"/>
-      <c r="D76" s="169"/>
-      <c r="E76" s="170"/>
+      <c r="C76" s="151"/>
+      <c r="D76" s="151"/>
+      <c r="E76" s="152"/>
       <c r="F76" s="57"/>
       <c r="G76" s="57"/>
       <c r="H76" s="57"/>
     </row>
     <row r="77" spans="1:8" ht="16.5" customHeight="1">
       <c r="A77" s="38"/>
-      <c r="B77" s="206" t="s">
+      <c r="B77" s="145" t="s">
         <v>40</v>
       </c>
-      <c r="C77" s="143" t="s">
-        <v>225</v>
-      </c>
-      <c r="D77" s="144"/>
-      <c r="E77" s="145"/>
+      <c r="C77" s="147" t="s">
+        <v>201</v>
+      </c>
+      <c r="D77" s="148"/>
+      <c r="E77" s="149"/>
       <c r="F77" s="57"/>
       <c r="G77" s="57"/>
       <c r="H77" s="57"/>
     </row>
     <row r="78" spans="1:8" ht="16.5" customHeight="1">
       <c r="A78" s="38"/>
-      <c r="B78" s="206" t="s">
+      <c r="B78" s="145" t="s">
         <v>24</v>
       </c>
-      <c r="C78" s="143" t="s">
-        <v>226</v>
-      </c>
-      <c r="D78" s="144"/>
-      <c r="E78" s="145"/>
+      <c r="C78" s="147" t="s">
+        <v>202</v>
+      </c>
+      <c r="D78" s="148"/>
+      <c r="E78" s="149"/>
       <c r="F78" s="57"/>
       <c r="G78" s="57"/>
       <c r="H78" s="57"/>
     </row>
     <row r="79" spans="1:8" ht="16.5" customHeight="1">
       <c r="A79" s="43"/>
-      <c r="B79" s="206" t="s">
+      <c r="B79" s="145" t="s">
         <v>41</v>
       </c>
-      <c r="C79" s="143" t="s">
-        <v>227</v>
-      </c>
-      <c r="D79" s="144"/>
-      <c r="E79" s="145"/>
+      <c r="C79" s="147" t="s">
+        <v>203</v>
+      </c>
+      <c r="D79" s="148"/>
+      <c r="E79" s="149"/>
       <c r="F79" s="57"/>
       <c r="G79" s="57"/>
       <c r="H79" s="57"/>
     </row>
     <row r="80" spans="1:8" ht="16.5" customHeight="1">
       <c r="A80" s="43"/>
-      <c r="B80" s="206" t="s">
+      <c r="B80" s="145" t="s">
         <v>19</v>
       </c>
-      <c r="C80" s="143" t="s">
-        <v>228</v>
-      </c>
-      <c r="D80" s="144"/>
-      <c r="E80" s="145"/>
+      <c r="C80" s="147" t="s">
+        <v>204</v>
+      </c>
+      <c r="D80" s="148"/>
+      <c r="E80" s="149"/>
       <c r="F80" s="57"/>
       <c r="G80" s="57"/>
       <c r="H80" s="57"/>
     </row>
     <row r="81" spans="1:8" ht="16.5" customHeight="1">
       <c r="A81" s="43"/>
-      <c r="B81" s="206" t="s">
+      <c r="B81" s="145" t="s">
         <v>20</v>
       </c>
-      <c r="C81" s="143" t="s">
-        <v>229</v>
-      </c>
-      <c r="D81" s="144"/>
-      <c r="E81" s="145"/>
+      <c r="C81" s="147" t="s">
+        <v>205</v>
+      </c>
+      <c r="D81" s="148"/>
+      <c r="E81" s="149"/>
       <c r="F81" s="57"/>
       <c r="G81" s="57"/>
       <c r="H81" s="57"/>
@@ -6335,13 +6341,13 @@
     <row r="82" spans="1:8" ht="16.5" customHeight="1">
       <c r="A82" s="43"/>
       <c r="B82" s="46" t="s">
-        <v>220</v>
-      </c>
-      <c r="C82" s="143" t="s">
-        <v>230</v>
-      </c>
-      <c r="D82" s="144"/>
-      <c r="E82" s="145"/>
+        <v>196</v>
+      </c>
+      <c r="C82" s="147" t="s">
+        <v>206</v>
+      </c>
+      <c r="D82" s="148"/>
+      <c r="E82" s="149"/>
       <c r="F82" s="57"/>
       <c r="G82" s="57"/>
       <c r="H82" s="57"/>
@@ -6349,13 +6355,13 @@
     <row r="83" spans="1:8" ht="16.5" customHeight="1">
       <c r="A83" s="43"/>
       <c r="B83" s="49" t="s">
-        <v>221</v>
-      </c>
-      <c r="C83" s="143" t="s">
-        <v>231</v>
-      </c>
-      <c r="D83" s="144"/>
-      <c r="E83" s="145"/>
+        <v>197</v>
+      </c>
+      <c r="C83" s="147" t="s">
+        <v>207</v>
+      </c>
+      <c r="D83" s="148"/>
+      <c r="E83" s="149"/>
       <c r="F83" s="57"/>
       <c r="G83" s="57"/>
       <c r="H83" s="57"/>
@@ -6363,13 +6369,13 @@
     <row r="84" spans="1:8" ht="16.5" customHeight="1">
       <c r="A84" s="43"/>
       <c r="B84" s="49" t="s">
-        <v>222</v>
-      </c>
-      <c r="C84" s="143" t="s">
-        <v>232</v>
-      </c>
-      <c r="D84" s="144"/>
-      <c r="E84" s="145"/>
+        <v>198</v>
+      </c>
+      <c r="C84" s="147" t="s">
+        <v>208</v>
+      </c>
+      <c r="D84" s="148"/>
+      <c r="E84" s="149"/>
       <c r="F84" s="57"/>
       <c r="G84" s="57"/>
       <c r="H84" s="57"/>
@@ -6379,11 +6385,11 @@
       <c r="B85" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="C85" s="143" t="s">
+      <c r="C85" s="147" t="s">
         <v>75</v>
       </c>
-      <c r="D85" s="144"/>
-      <c r="E85" s="145"/>
+      <c r="D85" s="148"/>
+      <c r="E85" s="149"/>
       <c r="F85" s="57"/>
       <c r="G85" s="57"/>
       <c r="H85" s="57"/>
@@ -6391,13 +6397,13 @@
     <row r="86" spans="1:8" ht="16.5" customHeight="1">
       <c r="A86" s="43"/>
       <c r="B86" s="49" t="s">
-        <v>224</v>
-      </c>
-      <c r="C86" s="143" t="s">
-        <v>233</v>
-      </c>
-      <c r="D86" s="144"/>
-      <c r="E86" s="145"/>
+        <v>200</v>
+      </c>
+      <c r="C86" s="147" t="s">
+        <v>209</v>
+      </c>
+      <c r="D86" s="148"/>
+      <c r="E86" s="149"/>
       <c r="F86" s="57"/>
       <c r="G86" s="57"/>
       <c r="H86" s="57"/>
@@ -6407,50 +6413,57 @@
       <c r="B87" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="C87" s="143" t="s">
+      <c r="C87" s="147" t="s">
         <v>79</v>
       </c>
-      <c r="D87" s="144"/>
-      <c r="E87" s="145"/>
+      <c r="D87" s="148"/>
+      <c r="E87" s="149"/>
       <c r="F87" s="57"/>
       <c r="G87" s="57"/>
       <c r="H87" s="57"/>
     </row>
     <row r="88" spans="1:8">
       <c r="B88" s="46" t="s">
-        <v>223</v>
-      </c>
-      <c r="C88" s="143" t="s">
-        <v>234</v>
-      </c>
-      <c r="D88" s="144"/>
-      <c r="E88" s="145"/>
+        <v>199</v>
+      </c>
+      <c r="C88" s="147" t="s">
+        <v>210</v>
+      </c>
+      <c r="D88" s="148"/>
+      <c r="E88" s="149"/>
     </row>
   </sheetData>
   <mergeCells count="69">
-    <mergeCell ref="C86:E86"/>
-    <mergeCell ref="C87:E87"/>
-    <mergeCell ref="C88:E88"/>
-    <mergeCell ref="C81:E81"/>
-    <mergeCell ref="C82:E82"/>
-    <mergeCell ref="C83:E83"/>
-    <mergeCell ref="C84:E84"/>
-    <mergeCell ref="C85:E85"/>
-    <mergeCell ref="C75:E75"/>
-    <mergeCell ref="C77:E77"/>
-    <mergeCell ref="C78:E78"/>
-    <mergeCell ref="C79:E79"/>
-    <mergeCell ref="C80:E80"/>
-    <mergeCell ref="B76:E76"/>
-    <mergeCell ref="C73:E73"/>
-    <mergeCell ref="C74:E74"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="B67:E67"/>
-    <mergeCell ref="B69:E69"/>
-    <mergeCell ref="C68:E68"/>
-    <mergeCell ref="C70:E70"/>
-    <mergeCell ref="C71:E71"/>
-    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="B52:E52"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C22:E22"/>
     <mergeCell ref="C31:E31"/>
     <mergeCell ref="C24:E24"/>
     <mergeCell ref="C60:E60"/>
@@ -6467,36 +6480,29 @@
     <mergeCell ref="C39:E39"/>
     <mergeCell ref="C30:E30"/>
     <mergeCell ref="C48:E48"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="C54:E54"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="B52:E52"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C73:E73"/>
+    <mergeCell ref="C74:E74"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="B67:E67"/>
+    <mergeCell ref="B69:E69"/>
+    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="C70:E70"/>
+    <mergeCell ref="C71:E71"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C75:E75"/>
+    <mergeCell ref="C77:E77"/>
+    <mergeCell ref="C78:E78"/>
+    <mergeCell ref="C79:E79"/>
+    <mergeCell ref="C80:E80"/>
+    <mergeCell ref="B76:E76"/>
+    <mergeCell ref="C86:E86"/>
+    <mergeCell ref="C87:E87"/>
+    <mergeCell ref="C88:E88"/>
+    <mergeCell ref="C81:E81"/>
+    <mergeCell ref="C82:E82"/>
+    <mergeCell ref="C83:E83"/>
+    <mergeCell ref="C84:E84"/>
+    <mergeCell ref="C85:E85"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6511,10 +6517,10 @@
   <sheetPr codeName="Hoja2">
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A3:Y46"/>
+  <dimension ref="A3:Y48"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="H24" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView showGridLines="0" topLeftCell="A27" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -6535,90 +6541,90 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:25" ht="18" customHeight="1">
-      <c r="B3" s="176" t="s">
-        <v>204</v>
-      </c>
-      <c r="C3" s="176"/>
-      <c r="D3" s="176"/>
-      <c r="E3" s="176"/>
-      <c r="F3" s="176"/>
-      <c r="G3" s="176"/>
-      <c r="H3" s="176"/>
-      <c r="I3" s="176"/>
-      <c r="J3" s="176"/>
-      <c r="K3" s="176"/>
-      <c r="L3" s="176"/>
-      <c r="M3" s="176"/>
-      <c r="N3" s="176"/>
+      <c r="B3" s="179" t="s">
+        <v>182</v>
+      </c>
+      <c r="C3" s="179"/>
+      <c r="D3" s="179"/>
+      <c r="E3" s="179"/>
+      <c r="F3" s="179"/>
+      <c r="G3" s="179"/>
+      <c r="H3" s="179"/>
+      <c r="I3" s="179"/>
+      <c r="J3" s="179"/>
+      <c r="K3" s="179"/>
+      <c r="L3" s="179"/>
+      <c r="M3" s="179"/>
+      <c r="N3" s="179"/>
     </row>
     <row r="4" spans="2:25" ht="11.25" customHeight="1">
       <c r="B4" s="4"/>
     </row>
     <row r="5" spans="2:25" ht="15" customHeight="1"/>
     <row r="6" spans="2:25" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="B6" s="171" t="s">
+      <c r="B6" s="181" t="s">
         <v>167</v>
       </c>
-      <c r="C6" s="172"/>
-      <c r="D6" s="173" t="s">
+      <c r="C6" s="182"/>
+      <c r="D6" s="176" t="s">
         <v>168</v>
       </c>
-      <c r="E6" s="174"/>
-      <c r="F6" s="175"/>
-      <c r="G6" s="177"/>
-      <c r="H6" s="177"/>
+      <c r="E6" s="177"/>
+      <c r="F6" s="178"/>
+      <c r="G6" s="180"/>
+      <c r="H6" s="180"/>
       <c r="Y6" s="3"/>
     </row>
     <row r="7" spans="2:25" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="B7" s="171" t="s">
+      <c r="B7" s="181" t="s">
         <v>164</v>
       </c>
-      <c r="C7" s="172"/>
-      <c r="D7" s="173" t="s">
+      <c r="C7" s="182"/>
+      <c r="D7" s="176" t="s">
         <v>160</v>
       </c>
-      <c r="E7" s="174"/>
-      <c r="F7" s="175"/>
+      <c r="E7" s="177"/>
+      <c r="F7" s="178"/>
       <c r="Y7" s="3"/>
     </row>
     <row r="8" spans="2:25" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="B8" s="171" t="s">
+      <c r="B8" s="181" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="172"/>
-      <c r="D8" s="173" t="s">
+      <c r="C8" s="182"/>
+      <c r="D8" s="176" t="s">
         <v>169</v>
       </c>
-      <c r="E8" s="174"/>
-      <c r="F8" s="175"/>
+      <c r="E8" s="177"/>
+      <c r="F8" s="178"/>
       <c r="Y8" s="3"/>
     </row>
     <row r="9" spans="2:25" s="5" customFormat="1" ht="16.5" customHeight="1">
-      <c r="B9" s="171" t="s">
+      <c r="B9" s="181" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="172"/>
+      <c r="C9" s="182"/>
       <c r="D9" s="107">
         <v>42901</v>
       </c>
       <c r="E9" s="108" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="203">
+      <c r="F9" s="143">
         <v>42903</v>
       </c>
       <c r="Y9" s="3"/>
     </row>
     <row r="10" spans="2:25" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="B10" s="171" t="s">
+      <c r="B10" s="181" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="172"/>
-      <c r="D10" s="173" t="s">
-        <v>172</v>
-      </c>
-      <c r="E10" s="174"/>
-      <c r="F10" s="175"/>
+      <c r="C10" s="182"/>
+      <c r="D10" s="176" t="s">
+        <v>171</v>
+      </c>
+      <c r="E10" s="177"/>
+      <c r="F10" s="178"/>
       <c r="Y10" s="3"/>
     </row>
     <row r="11" spans="2:25" s="20" customFormat="1" ht="15" customHeight="1">
@@ -6636,10 +6642,10 @@
         <v>119</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>212</v>
+        <v>189</v>
       </c>
       <c r="E12" s="36" t="s">
-        <v>211</v>
+        <v>188</v>
       </c>
       <c r="F12" s="11" t="s">
         <v>155</v>
@@ -6677,10 +6683,10 @@
         <v>154</v>
       </c>
       <c r="D13" s="101" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E13" s="102" t="s">
-        <v>170</v>
+        <v>219</v>
       </c>
       <c r="F13" s="102" t="s">
         <v>168</v>
@@ -6691,7 +6697,7 @@
       <c r="H13" s="103">
         <v>42901</v>
       </c>
-      <c r="I13" s="203">
+      <c r="I13" s="143">
         <v>42903</v>
       </c>
       <c r="J13" s="128">
@@ -6700,7 +6706,7 @@
       <c r="K13" s="103">
         <v>42902</v>
       </c>
-      <c r="L13" s="203">
+      <c r="L13" s="143">
         <v>42904</v>
       </c>
       <c r="M13" s="128">
@@ -6716,10 +6722,10 @@
         <v>154</v>
       </c>
       <c r="D14" s="101" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E14" s="102" t="s">
-        <v>201</v>
+        <v>220</v>
       </c>
       <c r="F14" s="102" t="s">
         <v>160</v>
@@ -6730,7 +6736,7 @@
       <c r="H14" s="103">
         <v>42901</v>
       </c>
-      <c r="I14" s="203">
+      <c r="I14" s="143">
         <v>42903</v>
       </c>
       <c r="J14" s="128">
@@ -6739,7 +6745,7 @@
       <c r="K14" s="103">
         <v>42901</v>
       </c>
-      <c r="L14" s="203">
+      <c r="L14" s="143">
         <v>42904</v>
       </c>
       <c r="M14" s="128">
@@ -6755,10 +6761,10 @@
         <v>154</v>
       </c>
       <c r="D15" s="101" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E15" s="102" t="s">
-        <v>180</v>
+        <v>221</v>
       </c>
       <c r="F15" s="102" t="s">
         <v>168</v>
@@ -6769,7 +6775,7 @@
       <c r="H15" s="103">
         <v>42901</v>
       </c>
-      <c r="I15" s="203">
+      <c r="I15" s="143">
         <v>42903</v>
       </c>
       <c r="J15" s="128">
@@ -6778,8 +6784,8 @@
       <c r="K15" s="103">
         <v>42901</v>
       </c>
-      <c r="L15" s="203">
-        <v>42905</v>
+      <c r="L15" s="143">
+        <v>42904</v>
       </c>
       <c r="M15" s="128">
         <v>2</v>
@@ -6794,13 +6800,13 @@
         <v>154</v>
       </c>
       <c r="D16" s="101" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E16" s="102" t="s">
-        <v>181</v>
+        <v>222</v>
       </c>
       <c r="F16" s="102" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="G16" s="102" t="s">
         <v>160</v>
@@ -6808,7 +6814,7 @@
       <c r="H16" s="103">
         <v>42901</v>
       </c>
-      <c r="I16" s="203">
+      <c r="I16" s="143">
         <v>42903</v>
       </c>
       <c r="J16" s="128">
@@ -6817,7 +6823,7 @@
       <c r="K16" s="103">
         <v>42901</v>
       </c>
-      <c r="L16" s="203">
+      <c r="L16" s="143">
         <v>42904</v>
       </c>
       <c r="M16" s="128">
@@ -6833,10 +6839,10 @@
         <v>154</v>
       </c>
       <c r="D17" s="101" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E17" s="102" t="s">
-        <v>183</v>
+        <v>223</v>
       </c>
       <c r="F17" s="102" t="s">
         <v>160</v>
@@ -6847,7 +6853,7 @@
       <c r="H17" s="103">
         <v>42901</v>
       </c>
-      <c r="I17" s="203">
+      <c r="I17" s="143">
         <v>42903</v>
       </c>
       <c r="J17" s="128">
@@ -6856,7 +6862,7 @@
       <c r="K17" s="103">
         <v>42901</v>
       </c>
-      <c r="L17" s="203">
+      <c r="L17" s="143">
         <v>42904</v>
       </c>
       <c r="M17" s="128">
@@ -6872,13 +6878,13 @@
         <v>154</v>
       </c>
       <c r="D18" s="101" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E18" s="102" t="s">
-        <v>202</v>
+        <v>224</v>
       </c>
       <c r="F18" s="102" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="G18" s="102" t="s">
         <v>160</v>
@@ -6886,7 +6892,7 @@
       <c r="H18" s="103">
         <v>42901</v>
       </c>
-      <c r="I18" s="203">
+      <c r="I18" s="143">
         <v>42903</v>
       </c>
       <c r="J18" s="128">
@@ -6895,7 +6901,7 @@
       <c r="K18" s="103">
         <v>42901</v>
       </c>
-      <c r="L18" s="203">
+      <c r="L18" s="143">
         <v>42904</v>
       </c>
       <c r="M18" s="128">
@@ -6911,10 +6917,10 @@
         <v>154</v>
       </c>
       <c r="D19" s="101" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E19" s="102" t="s">
-        <v>185</v>
+        <v>225</v>
       </c>
       <c r="F19" s="102" t="s">
         <v>160</v>
@@ -6925,7 +6931,7 @@
       <c r="H19" s="103">
         <v>42901</v>
       </c>
-      <c r="I19" s="203">
+      <c r="I19" s="143">
         <v>42903</v>
       </c>
       <c r="J19" s="128">
@@ -6934,7 +6940,7 @@
       <c r="K19" s="103">
         <v>42901</v>
       </c>
-      <c r="L19" s="203">
+      <c r="L19" s="143">
         <v>42904</v>
       </c>
       <c r="M19" s="128">
@@ -6950,13 +6956,13 @@
         <v>154</v>
       </c>
       <c r="D20" s="101" t="s">
+        <v>178</v>
+      </c>
+      <c r="E20" s="102" t="s">
+        <v>226</v>
+      </c>
+      <c r="F20" s="102" t="s">
         <v>179</v>
-      </c>
-      <c r="E20" s="102" t="s">
-        <v>186</v>
-      </c>
-      <c r="F20" s="102" t="s">
-        <v>182</v>
       </c>
       <c r="G20" s="102" t="s">
         <v>160</v>
@@ -6964,7 +6970,7 @@
       <c r="H20" s="103">
         <v>42901</v>
       </c>
-      <c r="I20" s="203">
+      <c r="I20" s="143">
         <v>42903</v>
       </c>
       <c r="J20" s="128">
@@ -6973,7 +6979,7 @@
       <c r="K20" s="103">
         <v>42901</v>
       </c>
-      <c r="L20" s="203">
+      <c r="L20" s="143">
         <v>42904</v>
       </c>
       <c r="M20" s="128">
@@ -6989,13 +6995,13 @@
         <v>154</v>
       </c>
       <c r="D21" s="101" t="s">
+        <v>178</v>
+      </c>
+      <c r="E21" s="102" t="s">
+        <v>227</v>
+      </c>
+      <c r="F21" s="102" t="s">
         <v>179</v>
-      </c>
-      <c r="E21" s="102" t="s">
-        <v>187</v>
-      </c>
-      <c r="F21" s="102" t="s">
-        <v>182</v>
       </c>
       <c r="G21" s="102" t="s">
         <v>160</v>
@@ -7003,7 +7009,7 @@
       <c r="H21" s="103">
         <v>42901</v>
       </c>
-      <c r="I21" s="203">
+      <c r="I21" s="143">
         <v>42903</v>
       </c>
       <c r="J21" s="128">
@@ -7012,7 +7018,7 @@
       <c r="K21" s="103">
         <v>42901</v>
       </c>
-      <c r="L21" s="203">
+      <c r="L21" s="143">
         <v>42904</v>
       </c>
       <c r="M21" s="128">
@@ -7028,13 +7034,13 @@
         <v>154</v>
       </c>
       <c r="D22" s="101" t="s">
+        <v>178</v>
+      </c>
+      <c r="E22" s="102" t="s">
+        <v>228</v>
+      </c>
+      <c r="F22" s="102" t="s">
         <v>179</v>
-      </c>
-      <c r="E22" s="102" t="s">
-        <v>188</v>
-      </c>
-      <c r="F22" s="102" t="s">
-        <v>182</v>
       </c>
       <c r="G22" s="102" t="s">
         <v>160</v>
@@ -7042,7 +7048,7 @@
       <c r="H22" s="103">
         <v>42901</v>
       </c>
-      <c r="I22" s="203">
+      <c r="I22" s="143">
         <v>42903</v>
       </c>
       <c r="J22" s="128">
@@ -7051,7 +7057,7 @@
       <c r="K22" s="103">
         <v>42901</v>
       </c>
-      <c r="L22" s="203">
+      <c r="L22" s="143">
         <v>42904</v>
       </c>
       <c r="M22" s="128">
@@ -7059,7 +7065,7 @@
       </c>
       <c r="N22" s="104"/>
     </row>
-    <row r="23" spans="2:14" ht="24">
+    <row r="23" spans="2:14" ht="36">
       <c r="B23" s="37">
         <v>11</v>
       </c>
@@ -7067,13 +7073,13 @@
         <v>154</v>
       </c>
       <c r="D23" s="101" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E23" s="102" t="s">
-        <v>189</v>
+        <v>229</v>
       </c>
       <c r="F23" s="102" t="s">
-        <v>208</v>
+        <v>186</v>
       </c>
       <c r="G23" s="102" t="s">
         <v>160</v>
@@ -7081,7 +7087,7 @@
       <c r="H23" s="103">
         <v>42901</v>
       </c>
-      <c r="I23" s="203">
+      <c r="I23" s="143">
         <v>42903</v>
       </c>
       <c r="J23" s="128">
@@ -7090,7 +7096,7 @@
       <c r="K23" s="103">
         <v>42901</v>
       </c>
-      <c r="L23" s="203">
+      <c r="L23" s="143">
         <v>42904</v>
       </c>
       <c r="M23" s="128">
@@ -7106,13 +7112,13 @@
         <v>154</v>
       </c>
       <c r="D24" s="101" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E24" s="102" t="s">
-        <v>190</v>
+        <v>230</v>
       </c>
       <c r="F24" s="102" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="G24" s="102" t="s">
         <v>160</v>
@@ -7120,7 +7126,7 @@
       <c r="H24" s="103">
         <v>42901</v>
       </c>
-      <c r="I24" s="203">
+      <c r="I24" s="143">
         <v>42903</v>
       </c>
       <c r="J24" s="128">
@@ -7129,7 +7135,7 @@
       <c r="K24" s="103">
         <v>42901</v>
       </c>
-      <c r="L24" s="203">
+      <c r="L24" s="143">
         <v>42904</v>
       </c>
       <c r="M24" s="128">
@@ -7145,10 +7151,10 @@
         <v>154</v>
       </c>
       <c r="D25" s="101" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E25" s="102" t="s">
-        <v>191</v>
+        <v>231</v>
       </c>
       <c r="F25" s="102" t="s">
         <v>160</v>
@@ -7159,7 +7165,7 @@
       <c r="H25" s="103">
         <v>42901</v>
       </c>
-      <c r="I25" s="203">
+      <c r="I25" s="143">
         <v>42903</v>
       </c>
       <c r="J25" s="128">
@@ -7168,7 +7174,7 @@
       <c r="K25" s="103">
         <v>42901</v>
       </c>
-      <c r="L25" s="203">
+      <c r="L25" s="143">
         <v>42904</v>
       </c>
       <c r="M25" s="128">
@@ -7184,10 +7190,10 @@
         <v>154</v>
       </c>
       <c r="D26" s="101" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E26" s="102" t="s">
-        <v>192</v>
+        <v>232</v>
       </c>
       <c r="F26" s="102" t="s">
         <v>160</v>
@@ -7198,7 +7204,7 @@
       <c r="H26" s="103">
         <v>42901</v>
       </c>
-      <c r="I26" s="203">
+      <c r="I26" s="143">
         <v>42903</v>
       </c>
       <c r="J26" s="128">
@@ -7207,7 +7213,7 @@
       <c r="K26" s="103">
         <v>42901</v>
       </c>
-      <c r="L26" s="203">
+      <c r="L26" s="143">
         <v>42904</v>
       </c>
       <c r="M26" s="128">
@@ -7223,10 +7229,10 @@
         <v>154</v>
       </c>
       <c r="D27" s="101" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E27" s="102" t="s">
-        <v>193</v>
+        <v>233</v>
       </c>
       <c r="F27" s="102" t="s">
         <v>160</v>
@@ -7237,7 +7243,7 @@
       <c r="H27" s="103">
         <v>42901</v>
       </c>
-      <c r="I27" s="203">
+      <c r="I27" s="143">
         <v>42903</v>
       </c>
       <c r="J27" s="128">
@@ -7246,7 +7252,7 @@
       <c r="K27" s="103">
         <v>42901</v>
       </c>
-      <c r="L27" s="203">
+      <c r="L27" s="143">
         <v>42904</v>
       </c>
       <c r="M27" s="128">
@@ -7262,10 +7268,10 @@
         <v>154</v>
       </c>
       <c r="D28" s="101" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E28" s="102" t="s">
-        <v>194</v>
+        <v>234</v>
       </c>
       <c r="F28" s="102" t="s">
         <v>160</v>
@@ -7276,7 +7282,7 @@
       <c r="H28" s="103">
         <v>42901</v>
       </c>
-      <c r="I28" s="203">
+      <c r="I28" s="143">
         <v>42903</v>
       </c>
       <c r="J28" s="128">
@@ -7285,7 +7291,7 @@
       <c r="K28" s="103">
         <v>42901</v>
       </c>
-      <c r="L28" s="203">
+      <c r="L28" s="143">
         <v>42904</v>
       </c>
       <c r="M28" s="128">
@@ -7293,7 +7299,7 @@
       </c>
       <c r="N28" s="104"/>
     </row>
-    <row r="29" spans="2:14" ht="24">
+    <row r="29" spans="2:14" ht="36">
       <c r="B29" s="37">
         <v>17</v>
       </c>
@@ -7301,13 +7307,13 @@
         <v>154</v>
       </c>
       <c r="D29" s="101" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E29" s="102" t="s">
-        <v>195</v>
+        <v>235</v>
       </c>
       <c r="F29" s="102" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="G29" s="102" t="s">
         <v>160</v>
@@ -7315,7 +7321,7 @@
       <c r="H29" s="103">
         <v>42901</v>
       </c>
-      <c r="I29" s="203">
+      <c r="I29" s="143">
         <v>42903</v>
       </c>
       <c r="J29" s="128">
@@ -7324,7 +7330,7 @@
       <c r="K29" s="103">
         <v>42901</v>
       </c>
-      <c r="L29" s="203">
+      <c r="L29" s="143">
         <v>42904</v>
       </c>
       <c r="M29" s="128">
@@ -7343,10 +7349,10 @@
         <v>177</v>
       </c>
       <c r="E30" s="102" t="s">
-        <v>196</v>
+        <v>241</v>
       </c>
       <c r="F30" s="102" t="s">
-        <v>168</v>
+        <v>180</v>
       </c>
       <c r="G30" s="102" t="s">
         <v>160</v>
@@ -7354,20 +7360,20 @@
       <c r="H30" s="103">
         <v>42901</v>
       </c>
-      <c r="I30" s="203">
+      <c r="I30" s="143">
         <v>42903</v>
       </c>
       <c r="J30" s="128">
-        <v>2</v>
+        <v>1.3</v>
       </c>
       <c r="K30" s="103">
         <v>42901</v>
       </c>
-      <c r="L30" s="203">
+      <c r="L30" s="143">
         <v>42904</v>
       </c>
       <c r="M30" s="128">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="N30" s="104"/>
     </row>
@@ -7382,10 +7388,10 @@
         <v>177</v>
       </c>
       <c r="E31" s="102" t="s">
-        <v>197</v>
+        <v>242</v>
       </c>
       <c r="F31" s="102" t="s">
-        <v>168</v>
+        <v>180</v>
       </c>
       <c r="G31" s="102" t="s">
         <v>160</v>
@@ -7393,16 +7399,16 @@
       <c r="H31" s="103">
         <v>42901</v>
       </c>
-      <c r="I31" s="203">
+      <c r="I31" s="143">
         <v>42903</v>
       </c>
       <c r="J31" s="128">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="K31" s="103">
         <v>42901</v>
       </c>
-      <c r="L31" s="203">
+      <c r="L31" s="143">
         <v>42904</v>
       </c>
       <c r="M31" s="128">
@@ -7418,10 +7424,10 @@
         <v>154</v>
       </c>
       <c r="D32" s="101" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E32" s="102" t="s">
-        <v>198</v>
+        <v>236</v>
       </c>
       <c r="F32" s="102" t="s">
         <v>168</v>
@@ -7432,16 +7438,16 @@
       <c r="H32" s="103">
         <v>42901</v>
       </c>
-      <c r="I32" s="203">
+      <c r="I32" s="143">
         <v>42903</v>
       </c>
       <c r="J32" s="128">
-        <v>1.3</v>
+        <v>2</v>
       </c>
       <c r="K32" s="103">
         <v>42901</v>
       </c>
-      <c r="L32" s="203">
+      <c r="L32" s="143">
         <v>42904</v>
       </c>
       <c r="M32" s="128">
@@ -7450,7 +7456,6 @@
       <c r="N32" s="104"/>
     </row>
     <row r="33" spans="1:14" ht="24">
-      <c r="A33" s="10"/>
       <c r="B33" s="37">
         <v>21</v>
       </c>
@@ -7458,10 +7463,10 @@
         <v>154</v>
       </c>
       <c r="D33" s="101" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E33" s="102" t="s">
-        <v>199</v>
+        <v>237</v>
       </c>
       <c r="F33" s="102" t="s">
         <v>168</v>
@@ -7472,25 +7477,24 @@
       <c r="H33" s="103">
         <v>42901</v>
       </c>
-      <c r="I33" s="203">
+      <c r="I33" s="143">
         <v>42903</v>
       </c>
       <c r="J33" s="128">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="K33" s="103">
         <v>42901</v>
       </c>
-      <c r="L33" s="203">
+      <c r="L33" s="143">
         <v>42904</v>
       </c>
       <c r="M33" s="128">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="N33" s="104"/>
     </row>
     <row r="34" spans="1:14" ht="24">
-      <c r="A34" s="10"/>
       <c r="B34" s="37">
         <v>22</v>
       </c>
@@ -7498,10 +7502,10 @@
         <v>154</v>
       </c>
       <c r="D34" s="101" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="E34" s="102" t="s">
-        <v>200</v>
+        <v>238</v>
       </c>
       <c r="F34" s="102" t="s">
         <v>168</v>
@@ -7512,76 +7516,156 @@
       <c r="H34" s="103">
         <v>42901</v>
       </c>
-      <c r="I34" s="203">
+      <c r="I34" s="143">
         <v>42903</v>
       </c>
       <c r="J34" s="128">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="K34" s="103">
         <v>42901</v>
       </c>
-      <c r="L34" s="203">
+      <c r="L34" s="143">
         <v>42904</v>
       </c>
       <c r="M34" s="128">
+        <v>1.3</v>
+      </c>
+      <c r="N34" s="104"/>
+    </row>
+    <row r="35" spans="1:14" ht="24">
+      <c r="A35" s="10"/>
+      <c r="B35" s="37">
+        <v>23</v>
+      </c>
+      <c r="C35" s="101" t="s">
+        <v>154</v>
+      </c>
+      <c r="D35" s="101" t="s">
+        <v>176</v>
+      </c>
+      <c r="E35" s="102" t="s">
+        <v>239</v>
+      </c>
+      <c r="F35" s="102" t="s">
+        <v>168</v>
+      </c>
+      <c r="G35" s="102" t="s">
+        <v>160</v>
+      </c>
+      <c r="H35" s="103">
+        <v>42901</v>
+      </c>
+      <c r="I35" s="143">
+        <v>42903</v>
+      </c>
+      <c r="J35" s="128">
+        <v>1.3</v>
+      </c>
+      <c r="K35" s="103">
+        <v>42901</v>
+      </c>
+      <c r="L35" s="143">
+        <v>42904</v>
+      </c>
+      <c r="M35" s="128">
+        <v>1.3</v>
+      </c>
+      <c r="N35" s="104"/>
+    </row>
+    <row r="36" spans="1:14" ht="24">
+      <c r="A36" s="10"/>
+      <c r="B36" s="37">
+        <v>24</v>
+      </c>
+      <c r="C36" s="101" t="s">
+        <v>154</v>
+      </c>
+      <c r="D36" s="101" t="s">
+        <v>172</v>
+      </c>
+      <c r="E36" s="102" t="s">
+        <v>240</v>
+      </c>
+      <c r="F36" s="102" t="s">
+        <v>168</v>
+      </c>
+      <c r="G36" s="102" t="s">
+        <v>160</v>
+      </c>
+      <c r="H36" s="103">
+        <v>42901</v>
+      </c>
+      <c r="I36" s="143">
+        <v>42903</v>
+      </c>
+      <c r="J36" s="128">
+        <v>1.4</v>
+      </c>
+      <c r="K36" s="103">
+        <v>42901</v>
+      </c>
+      <c r="L36" s="143">
+        <v>42904</v>
+      </c>
+      <c r="M36" s="128">
         <v>0.3</v>
       </c>
-      <c r="N34" s="104"/>
-    </row>
-    <row r="35" spans="1:14">
-      <c r="B35" s="8"/>
-      <c r="J35" s="105">
-        <f>SUM(J13:J34)</f>
-        <v>30.2</v>
-      </c>
-      <c r="L35" s="106" t="s">
+      <c r="N36" s="104"/>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="B37" s="8"/>
+      <c r="J37" s="105">
+        <f>SUM(J13:J36)</f>
+        <v>32.800000000000004</v>
+      </c>
+      <c r="L37" s="106" t="s">
         <v>16</v>
       </c>
-      <c r="M35" s="105">
-        <f>SUM(M13:M34)</f>
-        <v>29.400000000000002</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14">
-      <c r="B36" s="8"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-    </row>
-    <row r="42" spans="1:14" ht="12.75" customHeight="1"/>
-    <row r="43" spans="1:14">
-      <c r="A43" s="10"/>
-    </row>
-    <row r="44" spans="1:14">
-      <c r="A44" s="10"/>
-    </row>
+      <c r="M37" s="105">
+        <f>SUM(M13:M36)</f>
+        <v>31.400000000000002</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="B38" s="8"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+    </row>
+    <row r="44" spans="1:14" ht="12.75" customHeight="1"/>
     <row r="45" spans="1:14">
       <c r="A45" s="10"/>
     </row>
-    <row r="46" spans="1:14" ht="12.75" customHeight="1"/>
+    <row r="46" spans="1:14">
+      <c r="A46" s="10"/>
+    </row>
+    <row r="47" spans="1:14">
+      <c r="A47" s="10"/>
+    </row>
+    <row r="48" spans="1:14" ht="12.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D10:F10"/>
     <mergeCell ref="D7:F7"/>
     <mergeCell ref="B3:N3"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="D6:F6"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D10:F10"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13:C34">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13:C36">
       <formula1>TipoProy</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D13:D34">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D13:D36">
       <formula1>f_depar</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E19:E34">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E19:E36">
       <formula1>IF(C19="Fast Track",e_fast,IF(C19="Configuraciones Tipo o Nuevas",e_tipo,IF(C19="Desarrollos Departamentales",e_depar,IF(C19="Desarrollos Adicionales ATIS",e_atis,IF(C19="Definición de Requerimientos",e_req,e_inci)))))</formula1>
     </dataValidation>
   </dataValidations>
@@ -7598,13 +7682,13 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja4"/>
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="5" ySplit="4" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="M25" sqref="M25"/>
+      <selection pane="bottomRight" activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="11.25"/>
@@ -7625,22 +7709,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="29" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A1" s="178" t="s">
+      <c r="A1" s="183" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="179"/>
-      <c r="C1" s="179"/>
-      <c r="D1" s="179"/>
-      <c r="E1" s="179"/>
-      <c r="F1" s="179"/>
-      <c r="G1" s="179"/>
-      <c r="H1" s="179"/>
-      <c r="I1" s="179"/>
-      <c r="J1" s="179"/>
-      <c r="K1" s="179"/>
-      <c r="L1" s="179"/>
-      <c r="M1" s="179"/>
-      <c r="N1" s="180"/>
+      <c r="B1" s="184"/>
+      <c r="C1" s="184"/>
+      <c r="D1" s="184"/>
+      <c r="E1" s="184"/>
+      <c r="F1" s="184"/>
+      <c r="G1" s="184"/>
+      <c r="H1" s="184"/>
+      <c r="I1" s="184"/>
+      <c r="J1" s="184"/>
+      <c r="K1" s="184"/>
+      <c r="L1" s="184"/>
+      <c r="M1" s="184"/>
+      <c r="N1" s="185"/>
     </row>
     <row r="2" spans="1:15" s="29" customFormat="1" ht="11.45" customHeight="1">
       <c r="A2" s="30"/>
@@ -7718,23 +7802,23 @@
         <v>1</v>
       </c>
       <c r="C5" s="111" t="str">
-        <f>VLOOKUP(B5,Planificación!$B$13:$E$81,2,FALSE)</f>
+        <f>VLOOKUP(B5,Planificación!$B$13:$E$83,2,FALSE)</f>
         <v>Desarrollo de Sistemas</v>
       </c>
       <c r="D5" s="112" t="str">
-        <f>VLOOKUP(B5,Planificación!$B$13:$E$81,4,FALSE)</f>
-        <v>Plan de proyecto</v>
+        <f>VLOOKUP(B5,Planificación!$B$13:$E$83,4,FALSE)</f>
+        <v>Plan de proyecto (PPROY)</v>
       </c>
       <c r="E5" s="111" t="str">
-        <f>VLOOKUP(B5,Planificación!$B$13:$G$81,5,FALSE)</f>
+        <f>VLOOKUP(B5,Planificación!$B$13:$G$83,5,FALSE)</f>
         <v>Miguel Cotrina</v>
       </c>
       <c r="F5" s="111" t="str">
-        <f>VLOOKUP(B5,Planificación!$B$13:$G$81,6,FALSE)</f>
+        <f>VLOOKUP(B5,Planificación!$B$13:$G$83,6,FALSE)</f>
         <v>Luis Torres</v>
       </c>
       <c r="G5" s="114" t="s">
-        <v>205</v>
+        <v>183</v>
       </c>
       <c r="H5" s="113" t="s">
         <v>148</v>
@@ -7765,23 +7849,23 @@
         <v>2</v>
       </c>
       <c r="C6" s="111" t="str">
-        <f>VLOOKUP(B6,Planificación!$B$13:$E$81,2,FALSE)</f>
+        <f>VLOOKUP(B6,Planificación!$B$13:$E$83,2,FALSE)</f>
         <v>Desarrollo de Sistemas</v>
       </c>
       <c r="D6" s="112" t="str">
-        <f>VLOOKUP(B6,Planificación!$B$13:$E$81,4,FALSE)</f>
-        <v>Acta de reuniones</v>
+        <f>VLOOKUP(B6,Planificación!$B$13:$E$83,4,FALSE)</f>
+        <v>Acta de reuniones (ARINT- AREXT)</v>
       </c>
       <c r="E6" s="111" t="str">
-        <f>VLOOKUP(B6,Planificación!$B$13:$F$81,5,FALSE)</f>
+        <f>VLOOKUP(B6,Planificación!$B$13:$F$83,5,FALSE)</f>
         <v>Luis Torres</v>
       </c>
       <c r="F6" s="111" t="str">
-        <f>VLOOKUP(B6,Planificación!$B$13:$G$81,6,FALSE)</f>
+        <f>VLOOKUP(B6,Planificación!$B$13:$G$83,6,FALSE)</f>
         <v>Miguel Cotrina</v>
       </c>
       <c r="G6" s="114" t="s">
-        <v>209</v>
+        <v>187</v>
       </c>
       <c r="H6" s="113"/>
       <c r="I6" s="113" t="s">
@@ -7805,23 +7889,23 @@
         <v>3</v>
       </c>
       <c r="C7" s="111" t="str">
-        <f>VLOOKUP(B7,Planificación!$B$13:$E$81,2,FALSE)</f>
+        <f>VLOOKUP(B7,Planificación!$B$13:$E$83,2,FALSE)</f>
         <v>Desarrollo de Sistemas</v>
       </c>
       <c r="D7" s="112" t="str">
-        <f>VLOOKUP(B7,Planificación!$B$13:$E$81,4,FALSE)</f>
-        <v>Cronograma de proyecto</v>
+        <f>VLOOKUP(B7,Planificación!$B$13:$E$83,4,FALSE)</f>
+        <v>Cronograma de proyecto (CPROY)</v>
       </c>
       <c r="E7" s="111" t="str">
-        <f>VLOOKUP(B7,Planificación!$B$13:$F$81,5,FALSE)</f>
+        <f>VLOOKUP(B7,Planificación!$B$13:$F$83,5,FALSE)</f>
         <v>Miguel Cotrina</v>
       </c>
       <c r="F7" s="111" t="str">
-        <f>VLOOKUP(B7,Planificación!$B$13:$G$81,6,FALSE)</f>
+        <f>VLOOKUP(B7,Planificación!$B$13:$G$83,6,FALSE)</f>
         <v>Luis Torres</v>
       </c>
       <c r="G7" s="114" t="s">
-        <v>241</v>
+        <v>215</v>
       </c>
       <c r="H7" s="113" t="s">
         <v>148</v>
@@ -7853,23 +7937,23 @@
         <v>4</v>
       </c>
       <c r="C8" s="111" t="str">
-        <f>VLOOKUP(B8,Planificación!$B$13:$E$81,2,FALSE)</f>
+        <f>VLOOKUP(B8,Planificación!$B$13:$E$83,2,FALSE)</f>
         <v>Desarrollo de Sistemas</v>
       </c>
       <c r="D8" s="112" t="str">
-        <f>VLOOKUP(B8,Planificación!$B$13:$E$81,4,FALSE)</f>
-        <v>Proceso de gestion de proyecto</v>
+        <f>VLOOKUP(B8,Planificación!$B$13:$E$83,4,FALSE)</f>
+        <v>Proceso de gestion de proyecto (PGPROY)</v>
       </c>
       <c r="E8" s="111" t="str">
-        <f>VLOOKUP(B8,Planificación!$B$13:$F$81,5,FALSE)</f>
+        <f>VLOOKUP(B8,Planificación!$B$13:$F$83,5,FALSE)</f>
         <v>Sebastian Diego</v>
       </c>
       <c r="F8" s="111" t="str">
-        <f>VLOOKUP(B8,Planificación!$B$13:$G$81,6,FALSE)</f>
+        <f>VLOOKUP(B8,Planificación!$B$13:$G$83,6,FALSE)</f>
         <v>Luis Torres</v>
       </c>
       <c r="G8" s="114" t="s">
-        <v>206</v>
+        <v>184</v>
       </c>
       <c r="H8" s="113" t="s">
         <v>148</v>
@@ -7878,7 +7962,7 @@
         <v>94</v>
       </c>
       <c r="J8" s="113" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K8" s="115"/>
       <c r="L8" s="116">
@@ -7893,7 +7977,7 @@
       </c>
       <c r="O8" s="132"/>
     </row>
-    <row r="9" spans="1:15" ht="24">
+    <row r="9" spans="1:15" ht="41.25" customHeight="1">
       <c r="A9" s="109">
         <v>5</v>
       </c>
@@ -7901,23 +7985,23 @@
         <v>5</v>
       </c>
       <c r="C9" s="111" t="str">
-        <f>VLOOKUP(B9,Planificación!$B$13:$E$81,2,FALSE)</f>
+        <f>VLOOKUP(B9,Planificación!$B$13:$E$83,2,FALSE)</f>
         <v>Desarrollo de Sistemas</v>
       </c>
       <c r="D9" s="112" t="str">
-        <f>VLOOKUP(B9,Planificación!$B$13:$E$81,4,FALSE)</f>
-        <v>Aceptacion de entregables</v>
+        <f>VLOOKUP(B9,Planificación!$B$13:$E$83,4,FALSE)</f>
+        <v>Aceptacion de entregables (ACENTRE)</v>
       </c>
       <c r="E9" s="111" t="str">
-        <f>VLOOKUP(B9,Planificación!$B$13:$F$81,5,FALSE)</f>
+        <f>VLOOKUP(B9,Planificación!$B$13:$F$83,5,FALSE)</f>
         <v>Luis Torres</v>
       </c>
       <c r="F9" s="111" t="str">
-        <f>VLOOKUP(B9,Planificación!$B$13:$G$81,6,FALSE)</f>
+        <f>VLOOKUP(B9,Planificación!$B$13:$G$83,6,FALSE)</f>
         <v>Miguel Cotrina</v>
       </c>
       <c r="G9" s="114" t="s">
-        <v>217</v>
+        <v>193</v>
       </c>
       <c r="H9" s="113" t="s">
         <v>37</v>
@@ -7949,23 +8033,23 @@
         <v>6</v>
       </c>
       <c r="C10" s="111" t="str">
-        <f>VLOOKUP(B10,Planificación!$B$13:$E$81,2,FALSE)</f>
+        <f>VLOOKUP(B10,Planificación!$B$13:$E$83,2,FALSE)</f>
         <v>Desarrollo de Sistemas</v>
       </c>
       <c r="D10" s="112" t="str">
-        <f>VLOOKUP(B10,Planificación!$B$13:$E$81,4,FALSE)</f>
-        <v>Avance Quincenales</v>
+        <f>VLOOKUP(B10,Planificación!$B$13:$E$83,4,FALSE)</f>
+        <v>Avance Quincenales (IAVQUI)</v>
       </c>
       <c r="E10" s="111" t="str">
-        <f>VLOOKUP(B10,Planificación!$B$13:$F$81,5,FALSE)</f>
+        <f>VLOOKUP(B10,Planificación!$B$13:$F$83,5,FALSE)</f>
         <v>Junio Trillo</v>
       </c>
       <c r="F10" s="111" t="str">
-        <f>VLOOKUP(B10,Planificación!$B$13:$G$81,6,FALSE)</f>
+        <f>VLOOKUP(B10,Planificación!$B$13:$G$83,6,FALSE)</f>
         <v>Luis Torres</v>
       </c>
       <c r="G10" s="114" t="s">
-        <v>207</v>
+        <v>185</v>
       </c>
       <c r="H10" s="113" t="s">
         <v>37</v>
@@ -7974,7 +8058,7 @@
         <v>94</v>
       </c>
       <c r="J10" s="113" t="s">
-        <v>208</v>
+        <v>186</v>
       </c>
       <c r="K10" s="115"/>
       <c r="L10" s="116">
@@ -7997,27 +8081,25 @@
         <v>7</v>
       </c>
       <c r="C11" s="111" t="str">
-        <f>VLOOKUP(B11,Planificación!$B$13:$E$81,2,FALSE)</f>
+        <f>VLOOKUP(B11,Planificación!$B$13:$E$83,2,FALSE)</f>
         <v>Desarrollo de Sistemas</v>
       </c>
       <c r="D11" s="112" t="str">
-        <f>VLOOKUP(B11,Planificación!$B$13:$E$81,4,FALSE)</f>
-        <v>Registro de riesgos</v>
+        <f>VLOOKUP(B11,Planificación!$B$13:$E$83,4,FALSE)</f>
+        <v>Registro de riesgos (REGRI)</v>
       </c>
       <c r="E11" s="111" t="str">
-        <f>VLOOKUP(B11,Planificación!$B$13:$F$81,5,FALSE)</f>
+        <f>VLOOKUP(B11,Planificación!$B$13:$F$83,5,FALSE)</f>
         <v>Luis Torres</v>
       </c>
       <c r="F11" s="111" t="str">
-        <f>VLOOKUP(B11,Planificación!$B$13:$G$81,6,FALSE)</f>
+        <f>VLOOKUP(B11,Planificación!$B$13:$G$83,6,FALSE)</f>
         <v>Miguel Cotrina</v>
       </c>
       <c r="G11" s="114" t="s">
-        <v>209</v>
-      </c>
-      <c r="H11" s="113" t="s">
-        <v>210</v>
-      </c>
+        <v>187</v>
+      </c>
+      <c r="H11" s="113"/>
       <c r="I11" s="113" t="s">
         <v>94</v>
       </c>
@@ -8031,7 +8113,7 @@
       </c>
       <c r="O11" s="132"/>
     </row>
-    <row r="12" spans="1:15" ht="24">
+    <row r="12" spans="1:15" ht="45.75" customHeight="1">
       <c r="A12" s="109">
         <v>8</v>
       </c>
@@ -8039,23 +8121,23 @@
         <v>8</v>
       </c>
       <c r="C12" s="111" t="str">
-        <f>VLOOKUP(B12,Planificación!$B$13:$E$81,2,FALSE)</f>
+        <f>VLOOKUP(B12,Planificación!$B$13:$E$83,2,FALSE)</f>
         <v>Desarrollo de Sistemas</v>
       </c>
       <c r="D12" s="112" t="str">
-        <f>VLOOKUP(B12,Planificación!$B$13:$E$81,4,FALSE)</f>
-        <v>Registro de Items de configuracion</v>
+        <f>VLOOKUP(B12,Planificación!$B$13:$E$83,4,FALSE)</f>
+        <v>Registro de Items de configuracion (REGITCON)</v>
       </c>
       <c r="E12" s="111" t="str">
-        <f>VLOOKUP(B12,Planificación!$B$13:$F$81,5,FALSE)</f>
+        <f>VLOOKUP(B12,Planificación!$B$13:$F$83,5,FALSE)</f>
         <v>Sebastian Diego</v>
       </c>
       <c r="F12" s="111" t="str">
-        <f>VLOOKUP(B12,Planificación!$B$13:$G$81,6,FALSE)</f>
+        <f>VLOOKUP(B12,Planificación!$B$13:$G$83,6,FALSE)</f>
         <v>Luis Torres</v>
       </c>
       <c r="G12" s="114" t="s">
-        <v>214</v>
+        <v>248</v>
       </c>
       <c r="H12" s="113" t="s">
         <v>148</v>
@@ -8064,7 +8146,7 @@
         <v>94</v>
       </c>
       <c r="J12" s="113" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="K12" s="115"/>
       <c r="L12" s="116">
@@ -8087,23 +8169,23 @@
         <v>9</v>
       </c>
       <c r="C13" s="111" t="str">
-        <f>VLOOKUP(B13,Planificación!$B$13:$E$81,2,FALSE)</f>
+        <f>VLOOKUP(B13,Planificación!$B$13:$E$83,2,FALSE)</f>
         <v>Desarrollo de Sistemas</v>
       </c>
       <c r="D13" s="112" t="str">
-        <f>VLOOKUP(B13,Planificación!$B$13:$E$81,4,FALSE)</f>
-        <v>Formato de solicitud de accesos</v>
+        <f>VLOOKUP(B13,Planificación!$B$13:$E$83,4,FALSE)</f>
+        <v>Formato de solicitud de accesos (SOLACC)</v>
       </c>
       <c r="E13" s="111" t="str">
-        <f>VLOOKUP(B13,Planificación!$B$13:$F$81,5,FALSE)</f>
+        <f>VLOOKUP(B13,Planificación!$B$13:$F$83,5,FALSE)</f>
         <v>Sebastian Diego</v>
       </c>
       <c r="F13" s="111" t="str">
-        <f>VLOOKUP(B13,Planificación!$B$13:$G$81,6,FALSE)</f>
+        <f>VLOOKUP(B13,Planificación!$B$13:$G$83,6,FALSE)</f>
         <v>Luis Torres</v>
       </c>
       <c r="G13" s="114" t="s">
-        <v>235</v>
+        <v>211</v>
       </c>
       <c r="H13" s="113" t="s">
         <v>37</v>
@@ -8112,7 +8194,7 @@
         <v>94</v>
       </c>
       <c r="J13" s="113" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="K13" s="115"/>
       <c r="L13" s="116">
@@ -8135,23 +8217,23 @@
         <v>10</v>
       </c>
       <c r="C14" s="111" t="str">
-        <f>VLOOKUP(B14,Planificación!$B$13:$E$81,2,FALSE)</f>
+        <f>VLOOKUP(B14,Planificación!$B$13:$E$83,2,FALSE)</f>
         <v>Desarrollo de Sistemas</v>
       </c>
       <c r="D14" s="112" t="str">
-        <f>VLOOKUP(B14,Planificación!$B$13:$E$81,4,FALSE)</f>
-        <v>Proceso de gestion de configuracion</v>
+        <f>VLOOKUP(B14,Planificación!$B$13:$E$83,4,FALSE)</f>
+        <v>Proceso de gestion de configuracion (PGC)</v>
       </c>
       <c r="E14" s="111" t="str">
-        <f>VLOOKUP(B14,Planificación!$B$13:$F$81,5,FALSE)</f>
+        <f>VLOOKUP(B14,Planificación!$B$13:$F$83,5,FALSE)</f>
         <v>Sebastian Diego</v>
       </c>
       <c r="F14" s="111" t="str">
-        <f>VLOOKUP(B14,Planificación!$B$13:$G$81,6,FALSE)</f>
+        <f>VLOOKUP(B14,Planificación!$B$13:$G$83,6,FALSE)</f>
         <v>Luis Torres</v>
       </c>
       <c r="G14" s="114" t="s">
-        <v>215</v>
+        <v>191</v>
       </c>
       <c r="H14" s="113" t="s">
         <v>37</v>
@@ -8160,7 +8242,7 @@
         <v>94</v>
       </c>
       <c r="J14" s="113" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="K14" s="115"/>
       <c r="L14" s="116">
@@ -8175,7 +8257,7 @@
       </c>
       <c r="O14" s="132"/>
     </row>
-    <row r="15" spans="1:15" ht="36">
+    <row r="15" spans="1:15" ht="49.5" customHeight="1">
       <c r="A15" s="109">
         <v>11</v>
       </c>
@@ -8183,23 +8265,23 @@
         <v>11</v>
       </c>
       <c r="C15" s="111" t="str">
-        <f>VLOOKUP(B15,Planificación!$B$13:$E$81,2,FALSE)</f>
+        <f>VLOOKUP(B15,Planificación!$B$13:$E$83,2,FALSE)</f>
         <v>Desarrollo de Sistemas</v>
       </c>
       <c r="D15" s="112" t="str">
-        <f>VLOOKUP(B15,Planificación!$B$13:$E$81,4,FALSE)</f>
-        <v>Ficha de métricas de índice de cambios en ítems de configuración</v>
+        <f>VLOOKUP(B15,Planificación!$B$13:$E$83,4,FALSE)</f>
+        <v>Ficha de métricas de índice de cambios en ítems de configuración (FMICIC)</v>
       </c>
       <c r="E15" s="111" t="str">
-        <f>VLOOKUP(B15,Planificación!$B$13:$F$81,5,FALSE)</f>
+        <f>VLOOKUP(B15,Planificación!$B$13:$F$83,5,FALSE)</f>
         <v>Junior Trillo</v>
       </c>
       <c r="F15" s="111" t="str">
-        <f>VLOOKUP(B15,Planificación!$B$13:$G$81,6,FALSE)</f>
+        <f>VLOOKUP(B15,Planificación!$B$13:$G$83,6,FALSE)</f>
         <v>Luis Torres</v>
       </c>
       <c r="G15" s="114" t="s">
-        <v>240</v>
+        <v>214</v>
       </c>
       <c r="H15" s="113" t="s">
         <v>148</v>
@@ -8208,7 +8290,7 @@
         <v>94</v>
       </c>
       <c r="J15" s="113" t="s">
-        <v>208</v>
+        <v>186</v>
       </c>
       <c r="K15" s="115"/>
       <c r="L15" s="116">
@@ -8223,7 +8305,7 @@
       </c>
       <c r="O15" s="132"/>
     </row>
-    <row r="16" spans="1:15" ht="36">
+    <row r="16" spans="1:15" ht="51" customHeight="1">
       <c r="A16" s="109">
         <v>12</v>
       </c>
@@ -8231,23 +8313,23 @@
         <v>12</v>
       </c>
       <c r="C16" s="111" t="str">
-        <f>VLOOKUP(B16,Planificación!$B$13:$E$81,2,FALSE)</f>
+        <f>VLOOKUP(B16,Planificación!$B$13:$E$83,2,FALSE)</f>
         <v>Desarrollo de Sistemas</v>
       </c>
       <c r="D16" s="112" t="str">
-        <f>VLOOKUP(B16,Planificación!$B$13:$E$81,4,FALSE)</f>
-        <v>Ficha de métricas de volatilidad de requerimientos</v>
+        <f>VLOOKUP(B16,Planificación!$B$13:$E$83,4,FALSE)</f>
+        <v xml:space="preserve"> Ficha de métricas de volatilidad de requerimientos (FMVREQM)</v>
       </c>
       <c r="E16" s="111" t="str">
-        <f>VLOOKUP(B16,Planificación!$B$13:$F$81,5,FALSE)</f>
+        <f>VLOOKUP(B16,Planificación!$B$13:$F$83,5,FALSE)</f>
         <v>Junio Trillo</v>
       </c>
       <c r="F16" s="111" t="str">
-        <f>VLOOKUP(B16,Planificación!$B$13:$G$81,6,FALSE)</f>
+        <f>VLOOKUP(B16,Planificación!$B$13:$G$83,6,FALSE)</f>
         <v>Luis Torres</v>
       </c>
       <c r="G16" s="114" t="s">
-        <v>216</v>
+        <v>192</v>
       </c>
       <c r="H16" s="113" t="s">
         <v>37</v>
@@ -8256,7 +8338,7 @@
         <v>94</v>
       </c>
       <c r="J16" s="113" t="s">
-        <v>208</v>
+        <v>186</v>
       </c>
       <c r="K16" s="115"/>
       <c r="L16" s="116">
@@ -8266,36 +8348,36 @@
         <v>42905</v>
       </c>
       <c r="N16" s="117">
-        <f t="shared" ref="N16:N22" si="1">IF(M16&gt;0,1,0)</f>
+        <f t="shared" ref="N16:N23" si="1">IF(M16&gt;0,1,0)</f>
         <v>1</v>
       </c>
       <c r="O16" s="132"/>
     </row>
-    <row r="17" spans="1:15" ht="36">
+    <row r="17" spans="1:15" ht="51" customHeight="1">
       <c r="A17" s="109">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B17" s="110">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17" s="111" t="str">
-        <f>VLOOKUP(B17,Planificación!$B$13:$E$81,2,FALSE)</f>
+        <f>VLOOKUP(B17,Planificación!$B$13:$E$83,2,FALSE)</f>
         <v>Desarrollo de Sistemas</v>
       </c>
       <c r="D17" s="112" t="str">
-        <f>VLOOKUP(B17,Planificación!$B$13:$E$81,4,FALSE)</f>
-        <v>Herramienta de gestión de aseguramiento de calidad</v>
+        <f>VLOOKUP(B17,Planificación!$B$13:$E$83,4,FALSE)</f>
+        <v>CheckList de aseguramiento de la calidad (CHKQA)</v>
       </c>
       <c r="E17" s="111" t="str">
-        <f>VLOOKUP(B17,Planificación!$B$13:$F$81,5,FALSE)</f>
+        <f>VLOOKUP(B17,Planificación!$B$13:$F$83,5,FALSE)</f>
         <v>Luis Torres</v>
       </c>
       <c r="F17" s="111" t="str">
-        <f>VLOOKUP(B17,Planificación!$B$13:$G$81,6,FALSE)</f>
+        <f>VLOOKUP(B17,Planificación!$B$13:$G$83,6,FALSE)</f>
         <v>Miguel Cotrina</v>
       </c>
       <c r="G17" s="114" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="H17" s="113" t="s">
         <v>148</v>
@@ -8311,7 +8393,7 @@
         <v>42903</v>
       </c>
       <c r="M17" s="116">
-        <v>42905</v>
+        <v>42904</v>
       </c>
       <c r="N17" s="117">
         <f t="shared" si="1"/>
@@ -8321,29 +8403,29 @@
     </row>
     <row r="18" spans="1:15" ht="48">
       <c r="A18" s="109">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" s="110">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18" s="111" t="str">
-        <f>VLOOKUP(B18,Planificación!$B$13:$E$81,2,FALSE)</f>
+        <f>VLOOKUP(B18,Planificación!$B$13:$E$83,2,FALSE)</f>
         <v>Desarrollo de Sistemas</v>
       </c>
       <c r="D18" s="112" t="str">
-        <f>VLOOKUP(B18,Planificación!$B$13:$E$81,4,FALSE)</f>
-        <v>Matriz de seguimiento de proyecto interno</v>
+        <f>VLOOKUP(B18,Planificación!$B$13:$E$83,4,FALSE)</f>
+        <v>Herramienta de gestión de aseguramiento de calidad (HGQA)</v>
       </c>
       <c r="E18" s="111" t="str">
-        <f>VLOOKUP(B18,Planificación!$B$13:$F$81,5,FALSE)</f>
+        <f>VLOOKUP(B18,Planificación!$B$13:$F$83,5,FALSE)</f>
         <v>Luis Torres</v>
       </c>
       <c r="F18" s="111" t="str">
-        <f>VLOOKUP(B18,Planificación!$B$13:$G$81,6,FALSE)</f>
+        <f>VLOOKUP(B18,Planificación!$B$13:$G$83,6,FALSE)</f>
         <v>Miguel Cotrina</v>
       </c>
       <c r="G18" s="114" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="H18" s="113" t="s">
         <v>148</v>
@@ -8367,31 +8449,31 @@
       </c>
       <c r="O18" s="132"/>
     </row>
-    <row r="19" spans="1:15" ht="37.5" customHeight="1">
+    <row r="19" spans="1:15" ht="36">
       <c r="A19" s="109">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" s="110">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C19" s="111" t="str">
-        <f>VLOOKUP(B19,Planificación!$B$13:$E$81,2,FALSE)</f>
+        <f>VLOOKUP(B19,Planificación!$B$13:$E$83,2,FALSE)</f>
         <v>Desarrollo de Sistemas</v>
       </c>
       <c r="D19" s="112" t="str">
-        <f>VLOOKUP(B19,Planificación!$B$13:$E$81,4,FALSE)</f>
-        <v>Proceso de aseguramiento de calidad</v>
+        <f>VLOOKUP(B19,Planificación!$B$13:$E$83,4,FALSE)</f>
+        <v>Matriz de seguimiento de proyecto interno (MSPQA)</v>
       </c>
       <c r="E19" s="111" t="str">
-        <f>VLOOKUP(B19,Planificación!$B$13:$F$81,5,FALSE)</f>
+        <f>VLOOKUP(B19,Planificación!$B$13:$F$83,5,FALSE)</f>
         <v>Luis Torres</v>
       </c>
       <c r="F19" s="111" t="str">
-        <f>VLOOKUP(B19,Planificación!$B$13:$G$81,6,FALSE)</f>
+        <f>VLOOKUP(B19,Planificación!$B$13:$G$83,6,FALSE)</f>
         <v>Miguel Cotrina</v>
       </c>
       <c r="G19" s="114" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="H19" s="113" t="s">
         <v>148</v>
@@ -8415,40 +8497,40 @@
       </c>
       <c r="O19" s="132"/>
     </row>
-    <row r="20" spans="1:15" ht="48">
+    <row r="20" spans="1:15" ht="37.5" customHeight="1">
       <c r="A20" s="109">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20" s="110">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C20" s="111" t="str">
-        <f>VLOOKUP(B20,Planificación!$B$13:$E$81,2,FALSE)</f>
+        <f>VLOOKUP(B20,Planificación!$B$13:$E$83,2,FALSE)</f>
         <v>Desarrollo de Sistemas</v>
       </c>
       <c r="D20" s="112" t="str">
-        <f>VLOOKUP(B20,Planificación!$B$13:$E$81,4,FALSE)</f>
-        <v>Fichas de métricas de numero de N conformidades QA del producto</v>
+        <f>VLOOKUP(B20,Planificación!$B$13:$E$83,4,FALSE)</f>
+        <v>Proceso de aseguramiento de calidad (PQA)</v>
       </c>
       <c r="E20" s="111" t="str">
-        <f>VLOOKUP(B20,Planificación!$B$13:$F$81,5,FALSE)</f>
-        <v>Junio Trillo</v>
+        <f>VLOOKUP(B20,Planificación!$B$13:$F$83,5,FALSE)</f>
+        <v>Luis Torres</v>
       </c>
       <c r="F20" s="111" t="str">
-        <f>VLOOKUP(B20,Planificación!$B$13:$G$81,6,FALSE)</f>
-        <v>Luis Torres</v>
+        <f>VLOOKUP(B20,Planificación!$B$13:$G$83,6,FALSE)</f>
+        <v>Miguel Cotrina</v>
       </c>
       <c r="G20" s="114" t="s">
-        <v>243</v>
+        <v>216</v>
       </c>
       <c r="H20" s="113" t="s">
-        <v>37</v>
+        <v>148</v>
       </c>
       <c r="I20" s="113" t="s">
         <v>94</v>
       </c>
       <c r="J20" s="113" t="s">
-        <v>208</v>
+        <v>160</v>
       </c>
       <c r="K20" s="115"/>
       <c r="L20" s="116">
@@ -8463,31 +8545,31 @@
       </c>
       <c r="O20" s="132"/>
     </row>
-    <row r="21" spans="1:15" ht="24">
+    <row r="21" spans="1:15" ht="57" customHeight="1">
       <c r="A21" s="109">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21" s="110">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C21" s="111" t="str">
-        <f>VLOOKUP(B21,Planificación!$B$13:$E$81,2,FALSE)</f>
+        <f>VLOOKUP(B21,Planificación!$B$13:$E$83,2,FALSE)</f>
         <v>Desarrollo de Sistemas</v>
       </c>
       <c r="D21" s="112" t="str">
-        <f>VLOOKUP(B21,Planificación!$B$13:$E$81,4,FALSE)</f>
-        <v>Solicitud de cambios a requerimientos</v>
+        <f>VLOOKUP(B21,Planificación!$B$13:$E$83,4,FALSE)</f>
+        <v>Fichas de métricas de numero de N conformidades QA del producto (FMNCONPRO)</v>
       </c>
       <c r="E21" s="111" t="str">
-        <f>VLOOKUP(B21,Planificación!$B$13:$F$81,5,FALSE)</f>
-        <v>Miguel Cotrina</v>
+        <f>VLOOKUP(B21,Planificación!$B$13:$F$83,5,FALSE)</f>
+        <v>Junio Trillo</v>
       </c>
       <c r="F21" s="111" t="str">
-        <f>VLOOKUP(B21,Planificación!$B$13:$G$81,6,FALSE)</f>
+        <f>VLOOKUP(B21,Planificación!$B$13:$G$83,6,FALSE)</f>
         <v>Luis Torres</v>
       </c>
       <c r="G21" s="114" t="s">
-        <v>244</v>
+        <v>217</v>
       </c>
       <c r="H21" s="113" t="s">
         <v>37</v>
@@ -8496,7 +8578,7 @@
         <v>94</v>
       </c>
       <c r="J21" s="113" t="s">
-        <v>168</v>
+        <v>186</v>
       </c>
       <c r="K21" s="115"/>
       <c r="L21" s="116">
@@ -8511,31 +8593,31 @@
       </c>
       <c r="O21" s="132"/>
     </row>
-    <row r="22" spans="1:15" ht="24">
+    <row r="22" spans="1:15" ht="39" customHeight="1">
       <c r="A22" s="109">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" s="110">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C22" s="111" t="str">
-        <f>VLOOKUP(B22,Planificación!$B$13:$E$81,2,FALSE)</f>
+        <f>VLOOKUP(B22,Planificación!$B$13:$E$83,2,FALSE)</f>
         <v>Desarrollo de Sistemas</v>
       </c>
       <c r="D22" s="112" t="str">
-        <f>VLOOKUP(B22,Planificación!$B$13:$E$81,4,FALSE)</f>
-        <v>Matriz de trazabilidad de requerimientos</v>
+        <f>VLOOKUP(B22,Planificación!$B$13:$E$83,4,FALSE)</f>
+        <v>Fichas de métricas de exposicion al riesgo (FMEXRI)</v>
       </c>
       <c r="E22" s="111" t="str">
-        <f>VLOOKUP(B22,Planificación!$B$13:$F$81,5,FALSE)</f>
-        <v>Miguel Cotrina</v>
+        <f>VLOOKUP(B22,Planificación!$B$13:$F$83,5,FALSE)</f>
+        <v>Junio Trillo</v>
       </c>
       <c r="F22" s="111" t="str">
-        <f>VLOOKUP(B22,Planificación!$B$13:$G$81,6,FALSE)</f>
+        <f>VLOOKUP(B22,Planificación!$B$13:$G$83,6,FALSE)</f>
         <v>Luis Torres</v>
       </c>
       <c r="G22" s="114" t="s">
-        <v>236</v>
+        <v>218</v>
       </c>
       <c r="H22" s="113" t="s">
         <v>37</v>
@@ -8559,34 +8641,34 @@
       </c>
       <c r="O22" s="132"/>
     </row>
-    <row r="23" spans="1:15" ht="24">
+    <row r="23" spans="1:15" ht="37.5" customHeight="1">
       <c r="A23" s="109">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23" s="110">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C23" s="111" t="str">
-        <f>VLOOKUP(B23,Planificación!$B$13:$E$81,2,FALSE)</f>
+        <f>VLOOKUP(B23,Planificación!$B$13:$E$83,2,FALSE)</f>
         <v>Desarrollo de Sistemas</v>
       </c>
       <c r="D23" s="112" t="str">
-        <f>VLOOKUP(B23,Planificación!$B$13:$E$81,4,FALSE)</f>
-        <v>Proceso de gestión de requerimientos</v>
+        <f>VLOOKUP(B23,Planificación!$B$13:$E$83,4,FALSE)</f>
+        <v>Tablero de metricas (TMETR)</v>
       </c>
       <c r="E23" s="111" t="str">
-        <f>VLOOKUP(B23,Planificación!$B$13:$F$81,5,FALSE)</f>
-        <v>Miguel Cotrina</v>
+        <f>VLOOKUP(B23,Planificación!$B$13:$F$83,5,FALSE)</f>
+        <v>Junio Trillo</v>
       </c>
       <c r="F23" s="111" t="str">
-        <f>VLOOKUP(B23,Planificación!$B$13:$G$81,6,FALSE)</f>
+        <f>VLOOKUP(B23,Planificación!$B$13:$G$83,6,FALSE)</f>
         <v>Luis Torres</v>
       </c>
       <c r="G23" s="114" t="s">
-        <v>239</v>
+        <v>212</v>
       </c>
       <c r="H23" s="113" t="s">
-        <v>148</v>
+        <v>37</v>
       </c>
       <c r="I23" s="113" t="s">
         <v>94</v>
@@ -8602,82 +8684,86 @@
         <v>42905</v>
       </c>
       <c r="N23" s="117">
-        <f t="shared" ref="N23:N25" si="2">IF(M23&gt;0,1,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="O23" s="132"/>
     </row>
-    <row r="24" spans="1:15" ht="24">
+    <row r="24" spans="1:15" ht="36">
       <c r="A24" s="109">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B24" s="110">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C24" s="111" t="str">
-        <f>VLOOKUP(B24,Planificación!$B$13:$E$81,2,FALSE)</f>
+        <f>VLOOKUP(B24,Planificación!$B$13:$E$83,2,FALSE)</f>
         <v>Desarrollo de Sistemas</v>
       </c>
       <c r="D24" s="112" t="str">
-        <f>VLOOKUP(B24,Planificación!$B$13:$E$81,4,FALSE)</f>
-        <v>Registro de cambios a requerimientos</v>
+        <f>VLOOKUP(B24,Planificación!$B$13:$E$83,4,FALSE)</f>
+        <v>Solicitud de cambios a requerimientos (SOLCREQ)</v>
       </c>
       <c r="E24" s="111" t="str">
-        <f>VLOOKUP(B24,Planificación!$B$13:$F$81,5,FALSE)</f>
+        <f>VLOOKUP(B24,Planificación!$B$13:$F$83,5,FALSE)</f>
         <v>Miguel Cotrina</v>
       </c>
       <c r="F24" s="111" t="str">
-        <f>VLOOKUP(B24,Planificación!$B$13:$G$81,6,FALSE)</f>
+        <f>VLOOKUP(B24,Planificación!$B$13:$G$83,6,FALSE)</f>
         <v>Luis Torres</v>
       </c>
       <c r="G24" s="114" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="H24" s="113" t="s">
-        <v>210</v>
+        <v>148</v>
       </c>
       <c r="I24" s="113" t="s">
         <v>94</v>
       </c>
-      <c r="J24" s="113"/>
+      <c r="J24" s="113" t="s">
+        <v>168</v>
+      </c>
       <c r="K24" s="115"/>
-      <c r="L24" s="116"/>
-      <c r="M24" s="116"/>
+      <c r="L24" s="116">
+        <v>42903</v>
+      </c>
+      <c r="M24" s="116">
+        <v>42905</v>
+      </c>
       <c r="N24" s="117">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" ref="N24:N26" si="2">IF(M24&gt;0,1,0)</f>
+        <v>1</v>
       </c>
       <c r="O24" s="132"/>
     </row>
-    <row r="25" spans="1:15" ht="24">
+    <row r="25" spans="1:15" ht="36">
       <c r="A25" s="109">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B25" s="110">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C25" s="111" t="str">
-        <f>VLOOKUP(B25,Planificación!$B$13:$E$81,2,FALSE)</f>
+        <f>VLOOKUP(B25,Planificación!$B$13:$E$83,2,FALSE)</f>
         <v>Desarrollo de Sistemas</v>
       </c>
       <c r="D25" s="112" t="str">
-        <f>VLOOKUP(B25,Planificación!$B$13:$E$81,4,FALSE)</f>
-        <v>Lista maestra de requerimientos</v>
+        <f>VLOOKUP(B25,Planificación!$B$13:$E$83,4,FALSE)</f>
+        <v>Matriz de trazabilidad de requerimientos (MTREQM)</v>
       </c>
       <c r="E25" s="111" t="str">
-        <f>VLOOKUP(B25,Planificación!$B$13:$F$81,5,FALSE)</f>
+        <f>VLOOKUP(B25,Planificación!$B$13:$F$83,5,FALSE)</f>
         <v>Miguel Cotrina</v>
       </c>
       <c r="F25" s="111" t="str">
-        <f>VLOOKUP(B25,Planificación!$B$13:$G$81,6,FALSE)</f>
+        <f>VLOOKUP(B25,Planificación!$B$13:$G$83,6,FALSE)</f>
         <v>Luis Torres</v>
       </c>
       <c r="G25" s="114" t="s">
-        <v>209</v>
-      </c>
-      <c r="H25" s="113" t="s">
-        <v>210</v>
-      </c>
+        <v>187</v>
+      </c>
+      <c r="H25" s="113"/>
       <c r="I25" s="113" t="s">
         <v>94</v>
       </c>
@@ -8691,14 +8777,150 @@
       </c>
       <c r="O25" s="132"/>
     </row>
-    <row r="26" spans="1:15">
-      <c r="A26" s="19"/>
-      <c r="B26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="L26" s="19"/>
-      <c r="M26" s="19"/>
-      <c r="N26" s="19"/>
+    <row r="26" spans="1:15" ht="36">
+      <c r="A26" s="109">
+        <v>22</v>
+      </c>
+      <c r="B26" s="110">
+        <v>22</v>
+      </c>
+      <c r="C26" s="111" t="str">
+        <f>VLOOKUP(B26,Planificación!$B$13:$E$83,2,FALSE)</f>
+        <v>Desarrollo de Sistemas</v>
+      </c>
+      <c r="D26" s="112" t="str">
+        <f>VLOOKUP(B26,Planificación!$B$13:$E$83,4,FALSE)</f>
+        <v>Proceso de gestión de requerimientos (PGREQM)</v>
+      </c>
+      <c r="E26" s="111" t="str">
+        <f>VLOOKUP(B26,Planificación!$B$13:$F$83,5,FALSE)</f>
+        <v>Miguel Cotrina</v>
+      </c>
+      <c r="F26" s="111" t="str">
+        <f>VLOOKUP(B26,Planificación!$B$13:$G$83,6,FALSE)</f>
+        <v>Luis Torres</v>
+      </c>
+      <c r="G26" s="114" t="s">
+        <v>246</v>
+      </c>
+      <c r="H26" s="113" t="s">
+        <v>37</v>
+      </c>
+      <c r="I26" s="113" t="s">
+        <v>94</v>
+      </c>
+      <c r="J26" s="113" t="s">
+        <v>168</v>
+      </c>
+      <c r="K26" s="115"/>
+      <c r="L26" s="116">
+        <v>42903</v>
+      </c>
+      <c r="M26" s="116">
+        <v>42905</v>
+      </c>
+      <c r="N26" s="117">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O26" s="132"/>
+    </row>
+    <row r="27" spans="1:15" ht="36">
+      <c r="A27" s="109">
+        <v>23</v>
+      </c>
+      <c r="B27" s="110">
+        <v>23</v>
+      </c>
+      <c r="C27" s="111" t="str">
+        <f>VLOOKUP(B27,Planificación!$B$13:$E$83,2,FALSE)</f>
+        <v>Desarrollo de Sistemas</v>
+      </c>
+      <c r="D27" s="112" t="str">
+        <f>VLOOKUP(B27,Planificación!$B$13:$E$83,4,FALSE)</f>
+        <v>Registro de cambios a requerimientos (RCREQM)</v>
+      </c>
+      <c r="E27" s="111" t="str">
+        <f>VLOOKUP(B27,Planificación!$B$13:$F$83,5,FALSE)</f>
+        <v>Miguel Cotrina</v>
+      </c>
+      <c r="F27" s="111" t="str">
+        <f>VLOOKUP(B27,Planificación!$B$13:$G$83,6,FALSE)</f>
+        <v>Luis Torres</v>
+      </c>
+      <c r="G27" s="114" t="s">
+        <v>245</v>
+      </c>
+      <c r="H27" s="113" t="s">
+        <v>37</v>
+      </c>
+      <c r="I27" s="113" t="s">
+        <v>94</v>
+      </c>
+      <c r="J27" s="113" t="s">
+        <v>168</v>
+      </c>
+      <c r="K27" s="115"/>
+      <c r="L27" s="116">
+        <v>42903</v>
+      </c>
+      <c r="M27" s="116">
+        <v>42905</v>
+      </c>
+      <c r="N27" s="117">
+        <f t="shared" ref="N27" si="3">IF(M27&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O27" s="132"/>
+    </row>
+    <row r="28" spans="1:15" ht="24">
+      <c r="A28" s="109">
+        <v>24</v>
+      </c>
+      <c r="B28" s="110">
+        <v>24</v>
+      </c>
+      <c r="C28" s="111" t="str">
+        <f>VLOOKUP(B28,Planificación!$B$13:$E$83,2,FALSE)</f>
+        <v>Desarrollo de Sistemas</v>
+      </c>
+      <c r="D28" s="112" t="str">
+        <f>VLOOKUP(B28,Planificación!$B$13:$E$83,4,FALSE)</f>
+        <v>Lista maestra de requerimientos (LMR)</v>
+      </c>
+      <c r="E28" s="111" t="str">
+        <f>VLOOKUP(B28,Planificación!$B$13:$F$83,5,FALSE)</f>
+        <v>Miguel Cotrina</v>
+      </c>
+      <c r="F28" s="111" t="str">
+        <f>VLOOKUP(B28,Planificación!$B$13:$G$83,6,FALSE)</f>
+        <v>Luis Torres</v>
+      </c>
+      <c r="G28" s="114" t="s">
+        <v>187</v>
+      </c>
+      <c r="H28" s="113"/>
+      <c r="I28" s="113" t="s">
+        <v>94</v>
+      </c>
+      <c r="J28" s="113"/>
+      <c r="K28" s="115"/>
+      <c r="L28" s="116"/>
+      <c r="M28" s="116"/>
+      <c r="N28" s="117">
+        <f t="shared" ref="N28" si="4">IF(M28&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O28" s="132"/>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="A29" s="19"/>
+      <c r="B29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="L29" s="19"/>
+      <c r="M29" s="19"/>
+      <c r="N29" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -8706,10 +8928,10 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H28">
       <formula1>TiposNC</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I28">
       <formula1>Origen</formula1>
     </dataValidation>
   </dataValidations>
@@ -8727,10 +8949,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja5"/>
-  <dimension ref="A2:K61"/>
+  <dimension ref="A2:K60"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -8745,82 +8967,82 @@
   <sheetData>
     <row r="2" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
       <c r="A2" s="13"/>
-      <c r="C2" s="194" t="s">
+      <c r="C2" s="186" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="194"/>
-      <c r="E2" s="194"/>
-      <c r="F2" s="194"/>
-      <c r="G2" s="194"/>
-      <c r="H2" s="194"/>
-      <c r="I2" s="194"/>
-      <c r="J2" s="194"/>
-      <c r="K2" s="194"/>
+      <c r="D2" s="186"/>
+      <c r="E2" s="186"/>
+      <c r="F2" s="186"/>
+      <c r="G2" s="186"/>
+      <c r="H2" s="186"/>
+      <c r="I2" s="186"/>
+      <c r="J2" s="186"/>
+      <c r="K2" s="186"/>
     </row>
     <row r="3" spans="1:11" s="2" customFormat="1" ht="16.5" customHeight="1">
       <c r="A3" s="14"/>
     </row>
     <row r="4" spans="1:11" s="2" customFormat="1">
       <c r="A4" s="14"/>
-      <c r="C4" s="195" t="s">
+      <c r="C4" s="187" t="s">
         <v>163</v>
       </c>
-      <c r="D4" s="195"/>
-      <c r="E4" s="184" t="str">
+      <c r="D4" s="187"/>
+      <c r="E4" s="188" t="str">
         <f>IF(Planificación!D6&lt;&gt;"",Planificación!D6,"")</f>
         <v>Miguel Cotrina</v>
       </c>
-      <c r="F4" s="185"/>
-      <c r="G4" s="185"/>
-      <c r="H4" s="185"/>
-      <c r="I4" s="186"/>
+      <c r="F4" s="189"/>
+      <c r="G4" s="189"/>
+      <c r="H4" s="189"/>
+      <c r="I4" s="190"/>
     </row>
     <row r="5" spans="1:11" s="2" customFormat="1">
       <c r="A5" s="14"/>
-      <c r="C5" s="196" t="str">
+      <c r="C5" s="191" t="str">
         <f>Planificación!B7</f>
         <v>Analista de Calidad</v>
       </c>
-      <c r="D5" s="197"/>
-      <c r="E5" s="184" t="str">
+      <c r="D5" s="192"/>
+      <c r="E5" s="188" t="str">
         <f>IF(Planificación!D7&lt;&gt;"",Planificación!D7,"")</f>
         <v>Luis Torres</v>
       </c>
-      <c r="F5" s="185"/>
-      <c r="G5" s="185"/>
-      <c r="H5" s="185"/>
-      <c r="I5" s="186"/>
+      <c r="F5" s="189"/>
+      <c r="G5" s="189"/>
+      <c r="H5" s="189"/>
+      <c r="I5" s="190"/>
     </row>
     <row r="6" spans="1:11" s="2" customFormat="1">
       <c r="A6" s="14"/>
-      <c r="C6" s="182" t="s">
+      <c r="C6" s="194" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="183"/>
-      <c r="E6" s="184" t="str">
+      <c r="D6" s="195"/>
+      <c r="E6" s="188" t="str">
         <f>IF(Planificación!D8&lt;&gt;"",Planificación!D8,"")</f>
         <v>Miguel Cotrina - Luis Torres</v>
       </c>
-      <c r="F6" s="185"/>
-      <c r="G6" s="185"/>
-      <c r="H6" s="185"/>
-      <c r="I6" s="186"/>
+      <c r="F6" s="189"/>
+      <c r="G6" s="189"/>
+      <c r="H6" s="189"/>
+      <c r="I6" s="190"/>
     </row>
     <row r="7" spans="1:11" s="2" customFormat="1" ht="24" customHeight="1">
       <c r="A7" s="14"/>
-      <c r="C7" s="188" t="s">
+      <c r="C7" s="197" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="188"/>
-      <c r="E7" s="189">
+      <c r="D7" s="197"/>
+      <c r="E7" s="198">
         <f>IF(Planificación!D9&lt;&gt;"",Planificación!D9,"")</f>
         <v>42901</v>
       </c>
-      <c r="F7" s="190"/>
-      <c r="G7" s="191" t="s">
+      <c r="F7" s="199"/>
+      <c r="G7" s="200" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="192"/>
+      <c r="H7" s="201"/>
       <c r="I7" s="118">
         <f>IF(Planificación!F9&lt;&gt;"",Planificación!F9,"")</f>
         <v>42903</v>
@@ -8828,24 +9050,24 @@
     </row>
     <row r="8" spans="1:11" s="2" customFormat="1">
       <c r="A8" s="14"/>
-      <c r="C8" s="188" t="s">
+      <c r="C8" s="197" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="193"/>
-      <c r="E8" s="184" t="str">
+      <c r="D8" s="202"/>
+      <c r="E8" s="188" t="str">
         <f>IF(Planificación!D10&lt;&gt;"",Planificación!D10,"")</f>
         <v>Mayo 2017 - Junio 2017</v>
       </c>
-      <c r="F8" s="185"/>
-      <c r="G8" s="185"/>
-      <c r="H8" s="185"/>
-      <c r="I8" s="186"/>
+      <c r="F8" s="189"/>
+      <c r="G8" s="189"/>
+      <c r="H8" s="189"/>
+      <c r="I8" s="190"/>
     </row>
     <row r="13" spans="1:11" ht="15">
-      <c r="C13" s="187" t="s">
+      <c r="C13" s="196" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="187"/>
+      <c r="D13" s="196"/>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
       <c r="G13" s="15"/>
@@ -8858,8 +9080,8 @@
         <v>40</v>
       </c>
       <c r="D14" s="119">
-        <f>COUNTA(Planificación!C13:C34)</f>
-        <v>22</v>
+        <f>COUNTA(Planificación!C13:C36)</f>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="14.25" customHeight="1">
@@ -8876,8 +9098,8 @@
         <v>41</v>
       </c>
       <c r="D16" s="119">
-        <f>COUNT(Planificación!L13:L34)</f>
-        <v>22</v>
+        <f>COUNT(Planificación!L13:L36)</f>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="3:5">
@@ -8929,10 +9151,10 @@
       <c r="E24" s="12"/>
     </row>
     <row r="26" spans="3:5" ht="15" customHeight="1">
-      <c r="C26" s="181" t="s">
+      <c r="C26" s="193" t="s">
         <v>39</v>
       </c>
-      <c r="D26" s="181"/>
+      <c r="D26" s="193"/>
     </row>
     <row r="27" spans="3:5">
       <c r="C27" s="34" t="s">
@@ -8947,8 +9169,8 @@
         <v>148</v>
       </c>
       <c r="D28" s="122">
-        <f>COUNTIF('Seguimiento de NC'!$H$5:$H$148,C28)</f>
-        <v>9</v>
+        <f>COUNTIF('Seguimiento de NC'!$H$5:$H$151,C28)</f>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="3:5">
@@ -8956,7 +9178,7 @@
         <v>149</v>
       </c>
       <c r="D29" s="122">
-        <f>COUNTIF('Seguimiento de NC'!$H$5:$H$148,C29)</f>
+        <f>COUNTIF('Seguimiento de NC'!$H$5:$H$151,C29)</f>
         <v>0</v>
       </c>
     </row>
@@ -8965,8 +9187,8 @@
         <v>37</v>
       </c>
       <c r="D30" s="122">
-        <f>COUNTIF('Seguimiento de NC'!$H$5:$H$148,C30)</f>
-        <v>8</v>
+        <f>COUNTIF('Seguimiento de NC'!$H$5:$H$151,C30)</f>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="3:5">
@@ -8979,124 +9201,115 @@
       </c>
     </row>
     <row r="32" spans="3:5">
-      <c r="C32" s="123" t="s">
-        <v>210</v>
-      </c>
-      <c r="D32" s="122">
-        <f>COUNTIF('Seguimiento de NC'!$H$5:$H$148,C32)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="3:4">
-      <c r="C33" s="124" t="s">
+      <c r="C32" s="124" t="s">
         <v>16</v>
       </c>
-      <c r="D33" s="125">
-        <f>SUM(D28:D32)</f>
+      <c r="D32" s="125">
+        <f>SUM(D28:D31)</f>
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="3:4" ht="15">
-      <c r="C39" s="181" t="s">
+    <row r="38" spans="3:4" ht="15">
+      <c r="C38" s="193" t="s">
         <v>107</v>
       </c>
-      <c r="D39" s="181"/>
+      <c r="D38" s="193"/>
+    </row>
+    <row r="39" spans="3:4">
+      <c r="C39" s="124" t="s">
+        <v>108</v>
+      </c>
+      <c r="D39" s="122">
+        <f>Planificación!J37</f>
+        <v>32.800000000000004</v>
+      </c>
     </row>
     <row r="40" spans="3:4">
       <c r="C40" s="124" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D40" s="122">
-        <f>Planificación!J35</f>
-        <v>30.2</v>
+        <f>Planificación!M37</f>
+        <v>31.400000000000002</v>
       </c>
     </row>
     <row r="41" spans="3:4">
       <c r="C41" s="124" t="s">
-        <v>109</v>
+        <v>16</v>
       </c>
       <c r="D41" s="122">
-        <f>Planificación!M35</f>
-        <v>29.400000000000002</v>
-      </c>
-    </row>
-    <row r="42" spans="3:4">
-      <c r="C42" s="124" t="s">
+        <f>D39-D40</f>
+        <v>1.4000000000000021</v>
+      </c>
+    </row>
+    <row r="55" spans="3:4" ht="15">
+      <c r="C55" s="193" t="s">
+        <v>147</v>
+      </c>
+      <c r="D55" s="193"/>
+    </row>
+    <row r="56" spans="3:4">
+      <c r="C56" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="D56" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="D42" s="122">
-        <f>D40-D41</f>
-        <v>0.79999999999999716</v>
-      </c>
-    </row>
-    <row r="56" spans="3:4" ht="15">
-      <c r="C56" s="181" t="s">
-        <v>147</v>
-      </c>
-      <c r="D56" s="181"/>
     </row>
     <row r="57" spans="3:4">
-      <c r="C57" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="D57" s="33" t="s">
-        <v>16</v>
+      <c r="C57" s="127" t="s">
+        <v>94</v>
+      </c>
+      <c r="D57" s="122">
+        <f>COUNTIF('Seguimiento de NC'!$I$5:$I$151,C57)</f>
+        <v>24</v>
       </c>
     </row>
     <row r="58" spans="3:4">
       <c r="C58" s="127" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D58" s="122">
-        <f>COUNTIF('Seguimiento de NC'!$I$5:$I$148,C58)</f>
-        <v>21</v>
+        <f>COUNTIF('Seguimiento de NC'!$I$5:$I$151,C58)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="3:4">
       <c r="C59" s="127" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D59" s="122">
-        <f>COUNTIF('Seguimiento de NC'!$I$5:$I$148,C59)</f>
+        <f>COUNTIF('Seguimiento de NC'!$I$5:$I$151,C59)</f>
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="3:4">
-      <c r="C60" s="127" t="s">
-        <v>97</v>
-      </c>
-      <c r="D60" s="122">
-        <f>COUNTIF('Seguimiento de NC'!$I$5:$I$148,C60)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="3:4">
-      <c r="C61" s="124" t="s">
+      <c r="C60" s="124" t="s">
         <v>16</v>
       </c>
-      <c r="D61" s="125">
-        <f>SUM(D58:D60)</f>
-        <v>21</v>
+      <c r="D60" s="125">
+        <f>SUM(D57:D59)</f>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:I6"/>
+    <mergeCell ref="E8:I8"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C26:D26"/>
     <mergeCell ref="C2:K2"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="E4:I4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="E5:I5"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:I6"/>
-    <mergeCell ref="E8:I8"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C26:D26"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -9105,7 +9318,7 @@
     <oddFooter xml:space="preserve">&amp;LRev. 1.0&amp;CFecha Efectiva: 16/06/2008&amp;RPágina &amp;P de &amp;N </oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="D40:D42 D14:D18 D30" unlockedFormula="1"/>
+    <ignoredError sqref="D39:D41 D14:D18 D30" unlockedFormula="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>
@@ -9117,7 +9330,7 @@
   <dimension ref="A2:K44"/>
   <sheetViews>
     <sheetView zoomScale="75" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -9170,7 +9383,7 @@
       <c r="H3" s="127" t="s">
         <v>112</v>
       </c>
-      <c r="J3" s="198" t="s">
+      <c r="J3" s="203" t="s">
         <v>112</v>
       </c>
       <c r="K3" s="140" t="s">
@@ -9178,11 +9391,11 @@
       </c>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="199" t="s">
+      <c r="A4" s="204" t="s">
         <v>154</v>
       </c>
       <c r="B4" s="137" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D4" s="127" t="s">
         <v>96</v>
@@ -9193,13 +9406,13 @@
       <c r="H4" s="127" t="s">
         <v>113</v>
       </c>
-      <c r="J4" s="198"/>
+      <c r="J4" s="203"/>
       <c r="K4" s="140" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="200"/>
+      <c r="A5" s="205"/>
       <c r="B5" s="138" t="s">
         <v>150</v>
       </c>
@@ -9212,13 +9425,13 @@
       <c r="H5" s="127" t="s">
         <v>154</v>
       </c>
-      <c r="J5" s="198"/>
+      <c r="J5" s="203"/>
       <c r="K5" s="140" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="200"/>
+      <c r="A6" s="205"/>
       <c r="B6" s="138" t="s">
         <v>151</v>
       </c>
@@ -9226,21 +9439,19 @@
         <v>37</v>
       </c>
       <c r="H6" s="127"/>
-      <c r="J6" s="198"/>
+      <c r="J6" s="203"/>
       <c r="K6" s="140" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="200"/>
+      <c r="A7" s="205"/>
       <c r="B7" s="138" t="s">
-        <v>174</v>
-      </c>
-      <c r="F7" s="204" t="s">
-        <v>210</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="F7" s="144"/>
       <c r="H7" s="127"/>
-      <c r="J7" s="198" t="s">
+      <c r="J7" s="203" t="s">
         <v>121</v>
       </c>
       <c r="K7" s="140" t="s">
@@ -9248,7 +9459,7 @@
       </c>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="200"/>
+      <c r="A8" s="205"/>
       <c r="B8" s="138" t="s">
         <v>152</v>
       </c>
@@ -9256,80 +9467,80 @@
         <v>36</v>
       </c>
       <c r="H8" s="127"/>
-      <c r="J8" s="198"/>
+      <c r="J8" s="203"/>
       <c r="K8" s="140" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="200"/>
+      <c r="A9" s="205"/>
       <c r="B9" s="138" t="s">
         <v>153</v>
       </c>
-      <c r="J9" s="198"/>
+      <c r="J9" s="203"/>
       <c r="K9" s="140" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="200"/>
+      <c r="A10" s="205"/>
       <c r="B10" s="138" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F10" s="133"/>
-      <c r="J10" s="198"/>
+      <c r="J10" s="203"/>
       <c r="K10" s="140" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="200"/>
+      <c r="A11" s="205"/>
       <c r="B11" s="138" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F11" s="133"/>
-      <c r="J11" s="198"/>
+      <c r="J11" s="203"/>
       <c r="K11" s="140" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="200"/>
-      <c r="B12" s="202" t="s">
+      <c r="A12" s="205"/>
+      <c r="B12" s="142" t="s">
+        <v>177</v>
+      </c>
+      <c r="F12" s="133"/>
+      <c r="J12" s="203"/>
+      <c r="K12" s="140"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="205"/>
+      <c r="B13" s="142" t="s">
         <v>178</v>
       </c>
-      <c r="F12" s="133"/>
-      <c r="J12" s="198"/>
-      <c r="K12" s="140"/>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="200"/>
-      <c r="B13" s="202" t="s">
-        <v>179</v>
-      </c>
       <c r="F13" s="133"/>
-      <c r="J13" s="198"/>
+      <c r="J13" s="203"/>
       <c r="K13" s="140"/>
     </row>
     <row r="14" spans="1:11" ht="12.75" customHeight="1" thickBot="1">
-      <c r="A14" s="201"/>
+      <c r="A14" s="206"/>
       <c r="B14" s="139" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F14" s="133"/>
-      <c r="J14" s="198"/>
+      <c r="J14" s="203"/>
       <c r="K14" s="140" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:11">
-      <c r="J15" s="198"/>
+      <c r="J15" s="203"/>
       <c r="K15" s="140" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:11">
-      <c r="J16" s="198" t="s">
+      <c r="J16" s="203" t="s">
         <v>114</v>
       </c>
       <c r="K16" s="140" t="s">
@@ -9337,61 +9548,61 @@
       </c>
     </row>
     <row r="17" spans="10:11">
-      <c r="J17" s="198"/>
+      <c r="J17" s="203"/>
       <c r="K17" s="140" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="18" spans="10:11">
-      <c r="J18" s="198"/>
+      <c r="J18" s="203"/>
       <c r="K18" s="140" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="19" spans="10:11">
-      <c r="J19" s="198"/>
+      <c r="J19" s="203"/>
       <c r="K19" s="140" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="20" spans="10:11">
-      <c r="J20" s="198"/>
+      <c r="J20" s="203"/>
       <c r="K20" s="140" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="21" spans="10:11">
-      <c r="J21" s="198"/>
+      <c r="J21" s="203"/>
       <c r="K21" s="140" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="22" spans="10:11">
-      <c r="J22" s="198"/>
+      <c r="J22" s="203"/>
       <c r="K22" s="140" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="23" spans="10:11">
-      <c r="J23" s="198"/>
+      <c r="J23" s="203"/>
       <c r="K23" s="140" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="24" spans="10:11">
-      <c r="J24" s="198"/>
+      <c r="J24" s="203"/>
       <c r="K24" s="140" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="25" spans="10:11">
-      <c r="J25" s="198"/>
+      <c r="J25" s="203"/>
       <c r="K25" s="140" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="26" spans="10:11">
-      <c r="J26" s="198" t="s">
+      <c r="J26" s="203" t="s">
         <v>115</v>
       </c>
       <c r="K26" s="140" t="s">
@@ -9399,43 +9610,43 @@
       </c>
     </row>
     <row r="27" spans="10:11">
-      <c r="J27" s="198"/>
+      <c r="J27" s="203"/>
       <c r="K27" s="140" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="28" spans="10:11">
-      <c r="J28" s="198"/>
+      <c r="J28" s="203"/>
       <c r="K28" s="140" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="29" spans="10:11">
-      <c r="J29" s="198"/>
+      <c r="J29" s="203"/>
       <c r="K29" s="140" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="30" spans="10:11">
-      <c r="J30" s="198"/>
+      <c r="J30" s="203"/>
       <c r="K30" s="140" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="31" spans="10:11">
-      <c r="J31" s="198"/>
+      <c r="J31" s="203"/>
       <c r="K31" s="140" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="32" spans="10:11">
-      <c r="J32" s="198"/>
+      <c r="J32" s="203"/>
       <c r="K32" s="140" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="33" spans="10:11">
-      <c r="J33" s="198" t="s">
+      <c r="J33" s="203" t="s">
         <v>116</v>
       </c>
       <c r="K33" s="140" t="s">
@@ -9443,31 +9654,31 @@
       </c>
     </row>
     <row r="34" spans="10:11">
-      <c r="J34" s="198"/>
+      <c r="J34" s="203"/>
       <c r="K34" s="140" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="35" spans="10:11">
-      <c r="J35" s="198"/>
+      <c r="J35" s="203"/>
       <c r="K35" s="140" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="36" spans="10:11">
-      <c r="J36" s="198"/>
+      <c r="J36" s="203"/>
       <c r="K36" s="140" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="37" spans="10:11">
-      <c r="J37" s="198"/>
+      <c r="J37" s="203"/>
       <c r="K37" s="140" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="38" spans="10:11">
-      <c r="J38" s="198" t="s">
+      <c r="J38" s="203" t="s">
         <v>117</v>
       </c>
       <c r="K38" s="140" t="s">
@@ -9475,37 +9686,37 @@
       </c>
     </row>
     <row r="39" spans="10:11">
-      <c r="J39" s="198"/>
+      <c r="J39" s="203"/>
       <c r="K39" s="140" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="40" spans="10:11">
-      <c r="J40" s="198"/>
+      <c r="J40" s="203"/>
       <c r="K40" s="140" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="41" spans="10:11">
-      <c r="J41" s="198"/>
+      <c r="J41" s="203"/>
       <c r="K41" s="140" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="42" spans="10:11">
-      <c r="J42" s="198"/>
+      <c r="J42" s="203"/>
       <c r="K42" s="140" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="43" spans="10:11">
-      <c r="J43" s="198"/>
+      <c r="J43" s="203"/>
       <c r="K43" s="140" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="44" spans="10:11">
-      <c r="J44" s="198"/>
+      <c r="J44" s="203"/>
       <c r="K44" s="140" t="s">
         <v>126</v>
       </c>

</xml_diff>